<commit_message>
feat: complete service revamp
</commit_message>
<xml_diff>
--- a/DRAFT TIMETABLE I SEM 2025 -26.xlsx
+++ b/DRAFT TIMETABLE I SEM 2025 -26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adalmia/Downloads/Timetable Creator/timetable_maker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481FB20A-B512-D545-A0A2-63E108F273E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7134ED82-0281-744B-8B79-A7D0CFD8B506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6978" uniqueCount="1798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6972" uniqueCount="1795">
   <si>
     <r>
       <rPr>
@@ -15063,16 +15063,6 @@
         <rFont val="Calibri"/>
         <family val="1"/>
       </rPr>
-      <t>3 4 5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
       <t>Joshua Kumar Saladi</t>
     </r>
   </si>
@@ -15114,16 +15104,6 @@
         <family val="1"/>
       </rPr>
       <t>Valmiki Ashwith Kumar</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>2 3 4</t>
     </r>
   </si>
   <si>
@@ -18286,16 +18266,6 @@
         <rFont val="Calibri"/>
         <family val="1"/>
       </rPr>
-      <t>6 7 8 9</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
       <t>S R Rashmi</t>
     </r>
   </si>
@@ -19460,9 +19430,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m\ d\ yy;@"/>
-  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -19633,9 +19600,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" indent="3"/>
     </xf>
@@ -19665,6 +19629,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -19972,8 +19939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1907"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A1402" workbookViewId="0">
+      <selection activeCell="L1433" sqref="L1433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -19992,21 +19959,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="23"/>
     </row>
     <row r="2" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -21275,7 +21242,7 @@
       <c r="J54" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K54" s="25">
+      <c r="K54" s="24">
         <v>678</v>
       </c>
       <c r="L54" s="13"/>
@@ -29722,7 +29689,7 @@
       <c r="J379" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="K379" s="25">
+      <c r="K379" s="24">
         <v>789</v>
       </c>
       <c r="L379" s="13"/>
@@ -29764,7 +29731,7 @@
       <c r="J381" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="K381" s="25">
+      <c r="K381" s="24">
         <v>789</v>
       </c>
       <c r="L381" s="13"/>
@@ -31318,7 +31285,7 @@
       <c r="B447" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="C447" s="16" t="s">
+      <c r="C447" s="15" t="s">
         <v>679</v>
       </c>
       <c r="D447" s="10">
@@ -38711,7 +38678,7 @@
       <c r="B740" s="8" t="s">
         <v>940</v>
       </c>
-      <c r="C740" s="17" t="s">
+      <c r="C740" s="16" t="s">
         <v>941</v>
       </c>
       <c r="D740" s="10">
@@ -57184,7 +57151,7 @@
       <c r="J1469" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="K1469" s="18">
+      <c r="K1469" s="17">
         <v>8</v>
       </c>
       <c r="L1469" s="14"/>
@@ -57672,8 +57639,8 @@
       <c r="J1485" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K1485" s="4" t="s">
-        <v>1399</v>
+      <c r="K1485" s="4">
+        <v>345</v>
       </c>
       <c r="L1485" s="13"/>
       <c r="M1485" s="13"/>
@@ -57687,7 +57654,7 @@
       <c r="F1486" s="13"/>
       <c r="G1486" s="13"/>
       <c r="H1486" s="1" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="I1486" s="13"/>
       <c r="J1486" s="13"/>
@@ -57706,7 +57673,7 @@
         <v>35</v>
       </c>
       <c r="H1487" s="1" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="I1487" s="4" t="s">
         <v>1398</v>
@@ -57714,8 +57681,8 @@
       <c r="J1487" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="K1487" s="4" t="s">
-        <v>1399</v>
+      <c r="K1487" s="4">
+        <v>345</v>
       </c>
       <c r="L1487" s="13"/>
       <c r="M1487" s="13"/>
@@ -57729,7 +57696,7 @@
       <c r="F1488" s="13"/>
       <c r="G1488" s="13"/>
       <c r="H1488" s="1" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="I1488" s="13"/>
       <c r="J1488" s="13"/>
@@ -57765,7 +57732,7 @@
         <v>39</v>
       </c>
       <c r="H1490" s="1" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="I1490" s="4" t="s">
         <v>1398</v>
@@ -57773,8 +57740,8 @@
       <c r="J1490" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K1490" s="4" t="s">
-        <v>1399</v>
+      <c r="K1490" s="4">
+        <v>345</v>
       </c>
       <c r="L1490" s="13"/>
       <c r="M1490" s="13"/>
@@ -57788,7 +57755,7 @@
       <c r="F1491" s="13"/>
       <c r="G1491" s="13"/>
       <c r="H1491" s="1" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="I1491" s="13"/>
       <c r="J1491" s="13"/>
@@ -57805,7 +57772,7 @@
       <c r="F1492" s="13"/>
       <c r="G1492" s="13"/>
       <c r="H1492" s="1" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="I1492" s="13"/>
       <c r="J1492" s="13"/>
@@ -57824,7 +57791,7 @@
         <v>43</v>
       </c>
       <c r="H1493" s="1" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="I1493" s="4" t="s">
         <v>1398</v>
@@ -57832,8 +57799,8 @@
       <c r="J1493" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K1493" s="4" t="s">
-        <v>1405</v>
+      <c r="K1493" s="4">
+        <v>234</v>
       </c>
       <c r="L1493" s="13"/>
       <c r="M1493" s="13"/>
@@ -57847,7 +57814,7 @@
       <c r="F1494" s="13"/>
       <c r="G1494" s="13"/>
       <c r="H1494" s="1" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="I1494" s="13"/>
       <c r="J1494" s="13"/>
@@ -57864,7 +57831,7 @@
       <c r="F1495" s="13"/>
       <c r="G1495" s="13"/>
       <c r="H1495" s="1" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="I1495" s="13"/>
       <c r="J1495" s="13"/>
@@ -57883,7 +57850,7 @@
         <v>46</v>
       </c>
       <c r="H1496" s="1" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="I1496" s="4" t="s">
         <v>1398</v>
@@ -57891,8 +57858,8 @@
       <c r="J1496" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K1496" s="4" t="s">
-        <v>1405</v>
+      <c r="K1496" s="4">
+        <v>234</v>
       </c>
       <c r="L1496" s="13"/>
       <c r="M1496" s="13"/>
@@ -57906,7 +57873,7 @@
       <c r="F1497" s="13"/>
       <c r="G1497" s="13"/>
       <c r="H1497" s="1" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="I1497" s="13"/>
       <c r="J1497" s="13"/>
@@ -57923,7 +57890,7 @@
       <c r="F1498" s="13"/>
       <c r="G1498" s="13"/>
       <c r="H1498" s="1" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="I1498" s="13"/>
       <c r="J1498" s="13"/>
@@ -57942,7 +57909,7 @@
         <v>50</v>
       </c>
       <c r="H1499" s="1" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="I1499" s="4" t="s">
         <v>1398</v>
@@ -57950,8 +57917,8 @@
       <c r="J1499" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K1499" s="15">
-        <v>40399</v>
+      <c r="K1499" s="25">
+        <v>8910</v>
       </c>
       <c r="L1499" s="13"/>
       <c r="M1499" s="13"/>
@@ -57965,7 +57932,7 @@
       <c r="F1500" s="13"/>
       <c r="G1500" s="13"/>
       <c r="H1500" s="1" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="I1500" s="13"/>
       <c r="J1500" s="13"/>
@@ -57982,7 +57949,7 @@
       <c r="F1501" s="13"/>
       <c r="G1501" s="13"/>
       <c r="H1501" s="1" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="I1501" s="13"/>
       <c r="J1501" s="13"/>
@@ -57995,7 +57962,7 @@
         <v>1083</v>
       </c>
       <c r="B1502" s="1" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="C1502" s="1" t="s">
         <v>442</v>
@@ -58013,7 +57980,7 @@
         <v>16</v>
       </c>
       <c r="H1502" s="1" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="I1502" s="4" t="s">
         <v>1099</v>
@@ -58042,7 +58009,7 @@
         <v>78</v>
       </c>
       <c r="H1503" s="1" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="I1503" s="4" t="s">
         <v>1063</v>
@@ -58094,7 +58061,7 @@
       <c r="F1505" s="13"/>
       <c r="G1505" s="13"/>
       <c r="H1505" s="1" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="I1505" s="13"/>
       <c r="J1505" s="13"/>
@@ -58111,7 +58078,7 @@
       <c r="F1506" s="13"/>
       <c r="G1506" s="13"/>
       <c r="H1506" s="1" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="I1506" s="13"/>
       <c r="J1506" s="13"/>
@@ -58130,7 +58097,7 @@
         <v>91</v>
       </c>
       <c r="H1507" s="1" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="I1507" s="4" t="s">
         <v>383</v>
@@ -58153,7 +58120,7 @@
       <c r="F1508" s="13"/>
       <c r="G1508" s="13"/>
       <c r="H1508" s="1" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="I1508" s="13"/>
       <c r="J1508" s="13"/>
@@ -58170,7 +58137,7 @@
       <c r="F1509" s="13"/>
       <c r="G1509" s="13"/>
       <c r="H1509" s="1" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="I1509" s="13"/>
       <c r="J1509" s="13"/>
@@ -58183,7 +58150,7 @@
         <v>1082</v>
       </c>
       <c r="B1510" s="1" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="C1510" s="1" t="s">
         <v>462</v>
@@ -58201,7 +58168,7 @@
         <v>16</v>
       </c>
       <c r="H1510" s="1" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="I1510" s="4" t="s">
         <v>1099</v>
@@ -58228,7 +58195,7 @@
       <c r="F1511" s="13"/>
       <c r="G1511" s="13"/>
       <c r="H1511" s="1" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="I1511" s="4" t="s">
         <v>1099</v>
@@ -58253,7 +58220,7 @@
         <v>78</v>
       </c>
       <c r="H1512" s="1" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="I1512" s="4" t="s">
         <v>1063</v>
@@ -58280,7 +58247,7 @@
       <c r="F1513" s="13"/>
       <c r="G1513" s="13"/>
       <c r="H1513" s="1" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="I1513" s="4" t="s">
         <v>1063</v>
@@ -58305,7 +58272,7 @@
         <v>82</v>
       </c>
       <c r="H1514" s="1" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="I1514" s="4" t="s">
         <v>319</v>
@@ -58328,7 +58295,7 @@
       <c r="F1515" s="13"/>
       <c r="G1515" s="13"/>
       <c r="H1515" s="1" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="I1515" s="13"/>
       <c r="J1515" s="13"/>
@@ -58345,7 +58312,7 @@
       <c r="F1516" s="13"/>
       <c r="G1516" s="13"/>
       <c r="H1516" s="1" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="I1516" s="13"/>
       <c r="J1516" s="13"/>
@@ -58387,7 +58354,7 @@
       <c r="F1518" s="13"/>
       <c r="G1518" s="13"/>
       <c r="H1518" s="1" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="I1518" s="13"/>
       <c r="J1518" s="13"/>
@@ -58404,7 +58371,7 @@
       <c r="F1519" s="13"/>
       <c r="G1519" s="13"/>
       <c r="H1519" s="1" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="I1519" s="13"/>
       <c r="J1519" s="13"/>
@@ -58417,10 +58384,10 @@
         <v>2394</v>
       </c>
       <c r="B1520" s="8" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="C1520" s="9" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="D1520" s="10">
         <v>2</v>
@@ -58435,7 +58402,7 @@
         <v>16</v>
       </c>
       <c r="H1520" s="8" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="I1520" s="4" t="s">
         <v>1099</v>
@@ -58464,7 +58431,7 @@
         <v>78</v>
       </c>
       <c r="H1521" s="1" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="I1521" s="4" t="s">
         <v>1063</v>
@@ -58493,7 +58460,7 @@
         <v>82</v>
       </c>
       <c r="H1522" s="1" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="I1522" s="4" t="s">
         <v>319</v>
@@ -58516,7 +58483,7 @@
       <c r="F1523" s="13"/>
       <c r="G1523" s="13"/>
       <c r="H1523" s="1" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="I1523" s="13"/>
       <c r="J1523" s="13"/>
@@ -58552,7 +58519,7 @@
         <v>91</v>
       </c>
       <c r="H1525" s="1" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="I1525" s="4" t="s">
         <v>1099</v>
@@ -58575,7 +58542,7 @@
       <c r="F1526" s="13"/>
       <c r="G1526" s="13"/>
       <c r="H1526" s="1" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="I1526" s="13"/>
       <c r="J1526" s="13"/>
@@ -58592,7 +58559,7 @@
       <c r="F1527" s="13"/>
       <c r="G1527" s="13"/>
       <c r="H1527" s="1" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="I1527" s="13"/>
       <c r="J1527" s="13"/>
@@ -58609,7 +58576,7 @@
       <c r="F1528" s="13"/>
       <c r="G1528" s="13"/>
       <c r="H1528" s="1" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="I1528" s="13"/>
       <c r="J1528" s="13"/>
@@ -58651,7 +58618,7 @@
       <c r="F1530" s="13"/>
       <c r="G1530" s="13"/>
       <c r="H1530" s="1" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="I1530" s="13"/>
       <c r="J1530" s="13"/>
@@ -58670,7 +58637,7 @@
         <v>35</v>
       </c>
       <c r="H1531" s="1" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="I1531" s="4" t="s">
         <v>909</v>
@@ -58693,7 +58660,7 @@
       <c r="F1532" s="13"/>
       <c r="G1532" s="13"/>
       <c r="H1532" s="1" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="I1532" s="13"/>
       <c r="J1532" s="13"/>
@@ -58710,7 +58677,7 @@
       <c r="F1533" s="13"/>
       <c r="G1533" s="13"/>
       <c r="H1533" s="1" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="I1533" s="13"/>
       <c r="J1533" s="13"/>
@@ -58729,7 +58696,7 @@
         <v>39</v>
       </c>
       <c r="H1534" s="1" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="I1534" s="4" t="s">
         <v>909</v>
@@ -58752,7 +58719,7 @@
       <c r="F1535" s="13"/>
       <c r="G1535" s="13"/>
       <c r="H1535" s="1" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="I1535" s="13"/>
       <c r="J1535" s="13"/>
@@ -58769,7 +58736,7 @@
       <c r="F1536" s="13"/>
       <c r="G1536" s="13"/>
       <c r="H1536" s="1" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="I1536" s="13"/>
       <c r="J1536" s="13"/>
@@ -58788,7 +58755,7 @@
         <v>43</v>
       </c>
       <c r="H1537" s="1" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="I1537" s="4" t="s">
         <v>909</v>
@@ -58811,7 +58778,7 @@
       <c r="F1538" s="13"/>
       <c r="G1538" s="13"/>
       <c r="H1538" s="1" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="I1538" s="13"/>
       <c r="J1538" s="13"/>
@@ -58841,10 +58808,10 @@
         <v>2396</v>
       </c>
       <c r="B1540" s="8" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="C1540" s="9" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="D1540" s="10">
         <v>3</v>
@@ -58886,7 +58853,7 @@
       <c r="F1541" s="13"/>
       <c r="G1541" s="13"/>
       <c r="H1541" s="1" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="I1541" s="4" t="s">
         <v>1099</v>
@@ -58911,7 +58878,7 @@
         <v>78</v>
       </c>
       <c r="H1542" s="1" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="I1542" s="4" t="s">
         <v>1063</v>
@@ -58938,7 +58905,7 @@
       <c r="F1543" s="13"/>
       <c r="G1543" s="13"/>
       <c r="H1543" s="1" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="I1543" s="4" t="s">
         <v>1063</v>
@@ -58963,7 +58930,7 @@
         <v>82</v>
       </c>
       <c r="H1544" s="1" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="I1544" s="4" t="s">
         <v>319</v>
@@ -58986,7 +58953,7 @@
       <c r="F1545" s="13"/>
       <c r="G1545" s="13"/>
       <c r="H1545" s="1" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="I1545" s="13"/>
       <c r="J1545" s="13"/>
@@ -59003,7 +58970,7 @@
       <c r="F1546" s="13"/>
       <c r="G1546" s="13"/>
       <c r="H1546" s="1" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="I1546" s="13"/>
       <c r="J1546" s="13"/>
@@ -59022,7 +58989,7 @@
         <v>91</v>
       </c>
       <c r="H1547" s="1" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="I1547" s="4" t="s">
         <v>259</v>
@@ -59045,7 +59012,7 @@
       <c r="F1548" s="13"/>
       <c r="G1548" s="13"/>
       <c r="H1548" s="1" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="I1548" s="13"/>
       <c r="J1548" s="13"/>
@@ -59062,7 +59029,7 @@
       <c r="F1549" s="13"/>
       <c r="G1549" s="13"/>
       <c r="H1549" s="1" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="I1549" s="13"/>
       <c r="J1549" s="13"/>
@@ -59081,7 +59048,7 @@
         <v>30</v>
       </c>
       <c r="H1550" s="1" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="I1550" s="4" t="s">
         <v>473</v>
@@ -59104,7 +59071,7 @@
       <c r="F1551" s="13"/>
       <c r="G1551" s="13"/>
       <c r="H1551" s="1" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="I1551" s="13"/>
       <c r="J1551" s="13"/>
@@ -59121,7 +59088,7 @@
       <c r="F1552" s="13"/>
       <c r="G1552" s="13"/>
       <c r="H1552" s="1" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="I1552" s="13"/>
       <c r="J1552" s="13"/>
@@ -59140,7 +59107,7 @@
         <v>35</v>
       </c>
       <c r="H1553" s="1" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="I1553" s="4" t="s">
         <v>473</v>
@@ -59163,7 +59130,7 @@
       <c r="F1554" s="13"/>
       <c r="G1554" s="13"/>
       <c r="H1554" s="1" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="I1554" s="13"/>
       <c r="J1554" s="13"/>
@@ -59199,7 +59166,7 @@
         <v>39</v>
       </c>
       <c r="H1556" s="1" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="I1556" s="4" t="s">
         <v>473</v>
@@ -59222,7 +59189,7 @@
       <c r="F1557" s="13"/>
       <c r="G1557" s="13"/>
       <c r="H1557" s="1" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="I1557" s="13"/>
       <c r="J1557" s="13"/>
@@ -59239,7 +59206,7 @@
       <c r="F1558" s="13"/>
       <c r="G1558" s="13"/>
       <c r="H1558" s="1" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="I1558" s="13"/>
       <c r="J1558" s="13"/>
@@ -59258,7 +59225,7 @@
         <v>43</v>
       </c>
       <c r="H1559" s="1" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="I1559" s="4" t="s">
         <v>473</v>
@@ -59281,7 +59248,7 @@
       <c r="F1560" s="13"/>
       <c r="G1560" s="13"/>
       <c r="H1560" s="1" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="I1560" s="13"/>
       <c r="J1560" s="13"/>
@@ -59298,7 +59265,7 @@
       <c r="F1561" s="13"/>
       <c r="G1561" s="13"/>
       <c r="H1561" s="1" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="I1561" s="13"/>
       <c r="J1561" s="13"/>
@@ -59311,7 +59278,7 @@
         <v>1663</v>
       </c>
       <c r="B1562" s="1" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="C1562" s="1" t="s">
         <v>466</v>
@@ -59340,10 +59307,10 @@
         <v>2401</v>
       </c>
       <c r="B1563" s="8" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="C1563" s="9" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="D1563" s="10">
         <v>3</v>
@@ -59358,7 +59325,7 @@
         <v>16</v>
       </c>
       <c r="H1563" s="8" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="I1563" s="4" t="s">
         <v>1099</v>
@@ -59416,7 +59383,7 @@
         <v>82</v>
       </c>
       <c r="H1565" s="1" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="I1565" s="4" t="s">
         <v>319</v>
@@ -59439,7 +59406,7 @@
       <c r="F1566" s="13"/>
       <c r="G1566" s="13"/>
       <c r="H1566" s="1" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="I1566" s="13"/>
       <c r="J1566" s="13"/>
@@ -59458,7 +59425,7 @@
         <v>91</v>
       </c>
       <c r="H1567" s="1" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="I1567" s="4" t="s">
         <v>259</v>
@@ -59511,10 +59478,10 @@
         <v>2403</v>
       </c>
       <c r="B1570" s="8" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="C1570" s="9" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="D1570" s="10">
         <v>2</v>
@@ -59529,7 +59496,7 @@
         <v>16</v>
       </c>
       <c r="H1570" s="8" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="I1570" s="4" t="s">
         <v>1099</v>
@@ -59558,7 +59525,7 @@
         <v>78</v>
       </c>
       <c r="H1571" s="1" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="I1571" s="4" t="s">
         <v>1063</v>
@@ -59587,7 +59554,7 @@
         <v>82</v>
       </c>
       <c r="H1572" s="1" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="I1572" s="4" t="s">
         <v>1099</v>
@@ -59610,7 +59577,7 @@
       <c r="F1573" s="13"/>
       <c r="G1573" s="13"/>
       <c r="H1573" s="1" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="I1573" s="13"/>
       <c r="J1573" s="13"/>
@@ -59627,7 +59594,7 @@
       <c r="F1574" s="13"/>
       <c r="G1574" s="13"/>
       <c r="H1574" s="1" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="I1574" s="13"/>
       <c r="J1574" s="13"/>
@@ -59646,7 +59613,7 @@
         <v>91</v>
       </c>
       <c r="H1575" s="1" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="I1575" s="4" t="s">
         <v>1063</v>
@@ -59669,7 +59636,7 @@
       <c r="F1576" s="13"/>
       <c r="G1576" s="13"/>
       <c r="H1576" s="1" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="I1576" s="13"/>
       <c r="J1576" s="13"/>
@@ -59686,7 +59653,7 @@
       <c r="F1577" s="13"/>
       <c r="G1577" s="13"/>
       <c r="H1577" s="1" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="I1577" s="13"/>
       <c r="J1577" s="13"/>
@@ -59705,7 +59672,7 @@
         <v>30</v>
       </c>
       <c r="H1578" s="1" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="I1578" s="4" t="s">
         <v>406</v>
@@ -59728,7 +59695,7 @@
       <c r="F1579" s="13"/>
       <c r="G1579" s="13"/>
       <c r="H1579" s="1" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="I1579" s="13"/>
       <c r="J1579" s="13"/>
@@ -59745,7 +59712,7 @@
       <c r="F1580" s="13"/>
       <c r="G1580" s="13"/>
       <c r="H1580" s="1" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="I1580" s="13"/>
       <c r="J1580" s="13"/>
@@ -59764,7 +59731,7 @@
         <v>35</v>
       </c>
       <c r="H1581" s="1" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="I1581" s="4" t="s">
         <v>406</v>
@@ -59787,7 +59754,7 @@
       <c r="F1582" s="13"/>
       <c r="G1582" s="13"/>
       <c r="H1582" s="1" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="I1582" s="13"/>
       <c r="J1582" s="13"/>
@@ -59804,7 +59771,7 @@
       <c r="F1583" s="13"/>
       <c r="G1583" s="13"/>
       <c r="H1583" s="1" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="I1583" s="13"/>
       <c r="J1583" s="13"/>
@@ -59823,7 +59790,7 @@
         <v>39</v>
       </c>
       <c r="H1584" s="1" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="I1584" s="4" t="s">
         <v>406</v>
@@ -59846,7 +59813,7 @@
       <c r="F1585" s="13"/>
       <c r="G1585" s="13"/>
       <c r="H1585" s="1" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="I1585" s="13"/>
       <c r="J1585" s="13"/>
@@ -59863,7 +59830,7 @@
       <c r="F1586" s="13"/>
       <c r="G1586" s="13"/>
       <c r="H1586" s="1" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="I1586" s="13"/>
       <c r="J1586" s="13"/>
@@ -59882,7 +59849,7 @@
         <v>43</v>
       </c>
       <c r="H1587" s="1" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="I1587" s="4" t="s">
         <v>406</v>
@@ -59905,7 +59872,7 @@
       <c r="F1588" s="13"/>
       <c r="G1588" s="13"/>
       <c r="H1588" s="1" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="I1588" s="13"/>
       <c r="J1588" s="13"/>
@@ -59922,7 +59889,7 @@
       <c r="F1589" s="13"/>
       <c r="G1589" s="13"/>
       <c r="H1589" s="1" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="I1589" s="13"/>
       <c r="J1589" s="13"/>
@@ -59935,10 +59902,10 @@
         <v>2404</v>
       </c>
       <c r="B1590" s="8" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="C1590" s="9" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="D1590" s="10">
         <v>2</v>
@@ -59953,7 +59920,7 @@
         <v>16</v>
       </c>
       <c r="H1590" s="8" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="I1590" s="4" t="s">
         <v>112</v>
@@ -59982,7 +59949,7 @@
         <v>82</v>
       </c>
       <c r="H1591" s="1" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="I1591" s="4" t="s">
         <v>18</v>
@@ -60007,7 +59974,7 @@
         <v>91</v>
       </c>
       <c r="H1592" s="1" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="I1592" s="4" t="s">
         <v>537</v>
@@ -60032,7 +59999,7 @@
         <v>94</v>
       </c>
       <c r="H1593" s="1" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="I1593" s="4" t="s">
         <v>310</v>
@@ -60057,7 +60024,7 @@
         <v>97</v>
       </c>
       <c r="H1594" s="1" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="I1594" s="4" t="s">
         <v>618</v>
@@ -60076,10 +60043,10 @@
         <v>2405</v>
       </c>
       <c r="B1595" s="8" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="C1595" s="9" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="D1595" s="10">
         <v>2</v>
@@ -60094,7 +60061,7 @@
         <v>16</v>
       </c>
       <c r="H1595" s="8" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="I1595" s="4" t="s">
         <v>1099</v>
@@ -60152,7 +60119,7 @@
         <v>82</v>
       </c>
       <c r="H1597" s="1" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="I1597" s="4" t="s">
         <v>537</v>
@@ -60175,7 +60142,7 @@
       <c r="F1598" s="13"/>
       <c r="G1598" s="13"/>
       <c r="H1598" s="1" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="I1598" s="13"/>
       <c r="J1598" s="13"/>
@@ -60194,7 +60161,7 @@
         <v>94</v>
       </c>
       <c r="H1599" s="1" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="I1599" s="4" t="s">
         <v>310</v>
@@ -60236,7 +60203,7 @@
         <v>97</v>
       </c>
       <c r="H1601" s="1" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="I1601" s="4" t="s">
         <v>618</v>
@@ -60272,10 +60239,10 @@
         <v>2408</v>
       </c>
       <c r="B1603" s="8" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="C1603" s="9" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="D1603" s="10">
         <v>3</v>
@@ -60290,7 +60257,7 @@
         <v>16</v>
       </c>
       <c r="H1603" s="8" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="I1603" s="4" t="s">
         <v>618</v>
@@ -60338,7 +60305,7 @@
         <v>1680</v>
       </c>
       <c r="B1605" s="8" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="C1605" s="8" t="s">
         <v>491</v>
@@ -60367,7 +60334,7 @@
         <v>1748</v>
       </c>
       <c r="B1606" s="8" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="C1606" s="8" t="s">
         <v>491</v>
@@ -60396,7 +60363,7 @@
         <v>1697</v>
       </c>
       <c r="B1607" s="1" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="C1607" s="1" t="s">
         <v>494</v>
@@ -60425,7 +60392,7 @@
         <v>1764</v>
       </c>
       <c r="B1608" s="1" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="C1608" s="1" t="s">
         <v>494</v>
@@ -60454,10 +60421,10 @@
         <v>2310</v>
       </c>
       <c r="B1609" s="8" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="C1609" s="9" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="D1609" s="10">
         <v>3</v>
@@ -60472,7 +60439,7 @@
         <v>16</v>
       </c>
       <c r="H1609" s="8" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="I1609" s="4" t="s">
         <v>99</v>
@@ -60499,7 +60466,7 @@
       <c r="F1610" s="13"/>
       <c r="G1610" s="13"/>
       <c r="H1610" s="1" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="I1610" s="4" t="s">
         <v>99</v>
@@ -60518,10 +60485,10 @@
         <v>1284</v>
       </c>
       <c r="B1611" s="8" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="C1611" s="9" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="D1611" s="10">
         <v>3</v>
@@ -60563,7 +60530,7 @@
       <c r="F1612" s="13"/>
       <c r="G1612" s="13"/>
       <c r="H1612" s="1" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="I1612" s="4" t="s">
         <v>108</v>
@@ -60582,10 +60549,10 @@
         <v>1286</v>
       </c>
       <c r="B1613" s="8" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="C1613" s="9" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="D1613" s="10">
         <v>3</v>
@@ -60600,7 +60567,7 @@
         <v>16</v>
       </c>
       <c r="H1613" s="8" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="I1613" s="4" t="s">
         <v>108</v>
@@ -60627,7 +60594,7 @@
       <c r="F1614" s="13"/>
       <c r="G1614" s="13"/>
       <c r="H1614" s="1" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="I1614" s="13"/>
       <c r="J1614" s="13"/>
@@ -60644,7 +60611,7 @@
       <c r="F1615" s="13"/>
       <c r="G1615" s="13"/>
       <c r="H1615" s="1" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="I1615" s="4" t="s">
         <v>108</v>
@@ -60667,7 +60634,7 @@
       <c r="F1616" s="13"/>
       <c r="G1616" s="13"/>
       <c r="H1616" s="1" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="I1616" s="13"/>
       <c r="J1616" s="13"/>
@@ -60680,10 +60647,10 @@
         <v>741</v>
       </c>
       <c r="B1617" s="8" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
       <c r="C1617" s="8" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="D1617" s="10">
         <v>2</v>
@@ -60698,7 +60665,7 @@
         <v>16</v>
       </c>
       <c r="H1617" s="8" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="I1617" s="4" t="s">
         <v>261</v>
@@ -60727,16 +60694,16 @@
         <v>30</v>
       </c>
       <c r="H1618" s="1" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="I1618" s="4" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="J1618" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="K1618" s="15">
-        <v>40399</v>
+      <c r="K1618" s="25">
+        <v>8910</v>
       </c>
       <c r="L1618" s="13"/>
       <c r="M1618" s="13"/>
@@ -60746,10 +60713,10 @@
         <v>322</v>
       </c>
       <c r="B1619" s="8" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="C1619" s="8" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="D1619" s="10">
         <v>3</v>
@@ -60791,7 +60758,7 @@
       <c r="F1620" s="13"/>
       <c r="G1620" s="13"/>
       <c r="H1620" s="1" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="I1620" s="4" t="s">
         <v>25</v>
@@ -60816,7 +60783,7 @@
         <v>30</v>
       </c>
       <c r="H1621" s="1" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="I1621" s="4" t="s">
         <v>605</v>
@@ -60839,7 +60806,7 @@
       <c r="F1622" s="13"/>
       <c r="G1622" s="13"/>
       <c r="H1622" s="1" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="I1622" s="4" t="s">
         <v>605</v>
@@ -60858,10 +60825,10 @@
         <v>2059</v>
       </c>
       <c r="B1623" s="8" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="C1623" s="8" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="D1623" s="10">
         <v>3</v>
@@ -60876,7 +60843,7 @@
         <v>16</v>
       </c>
       <c r="H1623" s="8" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="I1623" s="4" t="s">
         <v>103</v>
@@ -60908,7 +60875,7 @@
         <v>262</v>
       </c>
       <c r="I1624" s="4" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="J1624" s="4" t="s">
         <v>119</v>
@@ -60924,10 +60891,10 @@
         <v>262</v>
       </c>
       <c r="B1625" s="8" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="C1625" s="9" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="D1625" s="10">
         <v>3</v>
@@ -60942,7 +60909,7 @@
         <v>16</v>
       </c>
       <c r="H1625" s="8" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="I1625" s="4" t="s">
         <v>103</v>
@@ -60971,7 +60938,7 @@
         <v>30</v>
       </c>
       <c r="H1626" s="1" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="I1626" s="4" t="s">
         <v>406</v>
@@ -60990,10 +60957,10 @@
         <v>2098</v>
       </c>
       <c r="B1627" s="8" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
       <c r="C1627" s="9" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="D1627" s="10">
         <v>3</v>
@@ -61008,7 +60975,7 @@
         <v>16</v>
       </c>
       <c r="H1627" s="8" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="I1627" s="4" t="s">
         <v>25</v>
@@ -61035,7 +61002,7 @@
       <c r="F1628" s="13"/>
       <c r="G1628" s="13"/>
       <c r="H1628" s="1" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="I1628" s="4" t="s">
         <v>25</v>
@@ -61060,10 +61027,10 @@
         <v>30</v>
       </c>
       <c r="H1629" s="1" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="I1629" s="4" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="J1629" s="4" t="s">
         <v>210</v>
@@ -61083,7 +61050,7 @@
       <c r="F1630" s="13"/>
       <c r="G1630" s="13"/>
       <c r="H1630" s="1" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="I1630" s="13"/>
       <c r="J1630" s="13"/>
@@ -61096,10 +61063,10 @@
         <v>2079</v>
       </c>
       <c r="B1631" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="C1631" s="8" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="D1631" s="10">
         <v>3</v>
@@ -61114,7 +61081,7 @@
         <v>16</v>
       </c>
       <c r="H1631" s="8" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="I1631" s="4" t="s">
         <v>116</v>
@@ -61185,10 +61152,10 @@
         <v>875</v>
       </c>
       <c r="B1634" s="1" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="C1634" s="1" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="D1634" s="10">
         <v>2</v>
@@ -61203,7 +61170,7 @@
         <v>16</v>
       </c>
       <c r="H1634" s="1" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="I1634" s="4" t="s">
         <v>93</v>
@@ -61232,10 +61199,10 @@
         <v>30</v>
       </c>
       <c r="H1635" s="1" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="I1635" s="4" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="J1635" s="4" t="s">
         <v>41</v>
@@ -61255,10 +61222,10 @@
       <c r="F1636" s="13"/>
       <c r="G1636" s="13"/>
       <c r="H1636" s="1" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="I1636" s="4" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="J1636" s="4" t="s">
         <v>33</v>
@@ -61274,10 +61241,10 @@
         <v>740</v>
       </c>
       <c r="B1637" s="8" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="C1637" s="9" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="D1637" s="10">
         <v>3</v>
@@ -61292,7 +61259,7 @@
         <v>16</v>
       </c>
       <c r="H1637" s="8" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="I1637" s="4" t="s">
         <v>167</v>
@@ -61319,7 +61286,7 @@
       <c r="F1638" s="13"/>
       <c r="G1638" s="13"/>
       <c r="H1638" s="1" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="I1638" s="4" t="s">
         <v>167</v>
@@ -61344,13 +61311,13 @@
         <v>30</v>
       </c>
       <c r="H1639" s="1" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="I1639" s="4" t="s">
         <v>909</v>
       </c>
       <c r="J1639" s="4" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="K1639" s="12">
         <v>89</v>
@@ -61363,10 +61330,10 @@
         <v>742</v>
       </c>
       <c r="B1640" s="8" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="C1640" s="9" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="D1640" s="10">
         <v>3</v>
@@ -61381,7 +61348,7 @@
         <v>16</v>
       </c>
       <c r="H1640" s="8" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="I1640" s="4" t="s">
         <v>240</v>
@@ -61425,7 +61392,7 @@
       <c r="F1642" s="13"/>
       <c r="G1642" s="13"/>
       <c r="H1642" s="1" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="I1642" s="4" t="s">
         <v>240</v>
@@ -61467,10 +61434,10 @@
         <v>30</v>
       </c>
       <c r="H1644" s="1" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="I1644" s="4" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="J1644" s="4" t="s">
         <v>194</v>
@@ -61490,7 +61457,7 @@
       <c r="F1645" s="13"/>
       <c r="G1645" s="13"/>
       <c r="H1645" s="1" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="I1645" s="13"/>
       <c r="J1645" s="13"/>
@@ -61503,10 +61470,10 @@
         <v>743</v>
       </c>
       <c r="B1646" s="1" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="C1646" s="1" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="D1646" s="10">
         <v>3</v>
@@ -61521,7 +61488,7 @@
         <v>16</v>
       </c>
       <c r="H1646" s="1" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="I1646" s="4" t="s">
         <v>343</v>
@@ -61573,7 +61540,7 @@
       <c r="F1648" s="13"/>
       <c r="G1648" s="13"/>
       <c r="H1648" s="1" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="I1648" s="13"/>
       <c r="J1648" s="13"/>
@@ -61592,7 +61559,7 @@
         <v>35</v>
       </c>
       <c r="H1649" s="1" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="I1649" s="4" t="s">
         <v>884</v>
@@ -61611,10 +61578,10 @@
         <v>2064</v>
       </c>
       <c r="B1650" s="8" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="C1650" s="8" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
       <c r="D1650" s="10">
         <v>3</v>
@@ -61629,7 +61596,7 @@
         <v>16</v>
       </c>
       <c r="H1650" s="8" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="I1650" s="4" t="s">
         <v>787</v>
@@ -61727,7 +61694,7 @@
       <c r="F1654" s="13"/>
       <c r="G1654" s="13"/>
       <c r="H1654" s="1" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="I1654" s="13"/>
       <c r="J1654" s="13"/>
@@ -61740,10 +61707,10 @@
         <v>606</v>
       </c>
       <c r="B1655" s="1" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="C1655" s="1" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="D1655" s="10">
         <v>3</v>
@@ -61810,7 +61777,7 @@
       <c r="F1657" s="13"/>
       <c r="G1657" s="13"/>
       <c r="H1657" s="1" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="I1657" s="13"/>
       <c r="J1657" s="13"/>
@@ -61819,14 +61786,14 @@
       <c r="M1657" s="13"/>
     </row>
     <row r="1658" spans="1:13" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1658" s="19">
+      <c r="A1658" s="18">
         <v>744</v>
       </c>
-      <c r="B1658" s="20" t="s">
-        <v>1541</v>
+      <c r="B1658" s="19" t="s">
+        <v>1539</v>
       </c>
       <c r="C1658" s="1" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="D1658" s="10">
         <v>3</v>
@@ -61837,11 +61804,11 @@
       <c r="F1658" s="10">
         <v>5</v>
       </c>
-      <c r="G1658" s="21" t="s">
+      <c r="G1658" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H1658" s="20" t="s">
-        <v>1543</v>
+      <c r="H1658" s="19" t="s">
+        <v>1541</v>
       </c>
       <c r="I1658" s="4" t="s">
         <v>240</v>
@@ -61876,7 +61843,7 @@
         <v>954</v>
       </c>
       <c r="J1659" s="4" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
       <c r="K1659" s="12">
         <v>12</v>
@@ -61893,7 +61860,7 @@
       <c r="F1660" s="13"/>
       <c r="G1660" s="13"/>
       <c r="H1660" s="1" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="I1660" s="13"/>
       <c r="J1660" s="13"/>
@@ -61904,10 +61871,10 @@
     <row r="1661" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1661" s="14"/>
       <c r="B1661" s="1" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="C1661" s="9" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
       <c r="D1661" s="10">
         <v>2</v>
@@ -61951,10 +61918,10 @@
         <v>30</v>
       </c>
       <c r="H1662" s="1" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="I1662" s="4" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="J1662" s="4" t="s">
         <v>52</v>
@@ -61970,7 +61937,7 @@
         <v>1418</v>
       </c>
       <c r="B1663" s="8" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="C1663" s="9" t="s">
         <v>1288</v>
@@ -62011,10 +61978,10 @@
         <v>1024</v>
       </c>
       <c r="B1664" s="8" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="C1664" s="9" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="D1664" s="10">
         <v>3</v>
@@ -62029,7 +61996,7 @@
         <v>16</v>
       </c>
       <c r="H1664" s="8" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="I1664" s="4" t="s">
         <v>1063</v>
@@ -62056,7 +62023,7 @@
       <c r="F1665" s="13"/>
       <c r="G1665" s="13"/>
       <c r="H1665" s="1" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
       <c r="I1665" s="4" t="s">
         <v>1063</v>
@@ -62081,7 +62048,7 @@
         <v>82</v>
       </c>
       <c r="H1666" s="1" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
       <c r="I1666" s="4" t="s">
         <v>1063</v>
@@ -62100,10 +62067,10 @@
         <v>12545</v>
       </c>
       <c r="B1667" s="8" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="C1667" s="9" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="D1667" s="10">
         <v>3</v>
@@ -62118,7 +62085,7 @@
         <v>16</v>
       </c>
       <c r="H1667" s="8" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="I1667" s="4" t="s">
         <v>336</v>
@@ -62141,10 +62108,10 @@
         <v>2548</v>
       </c>
       <c r="B1668" s="8" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
       <c r="C1668" s="9" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="D1668" s="10">
         <v>3</v>
@@ -62186,7 +62153,7 @@
       <c r="F1669" s="13"/>
       <c r="G1669" s="13"/>
       <c r="H1669" s="1" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="I1669" s="4" t="s">
         <v>1024</v>
@@ -62205,10 +62172,10 @@
         <v>369</v>
       </c>
       <c r="B1670" s="1" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="C1670" s="1" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
       <c r="D1670" s="10">
         <v>3</v>
@@ -62252,10 +62219,10 @@
         <v>30</v>
       </c>
       <c r="H1671" s="1" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="I1671" s="4" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="J1671" s="4" t="s">
         <v>52</v>
@@ -62271,10 +62238,10 @@
         <v>649</v>
       </c>
       <c r="B1672" s="8" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="C1672" s="9" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="D1672" s="10">
         <v>3</v>
@@ -62318,7 +62285,7 @@
         <v>30</v>
       </c>
       <c r="H1673" s="1" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="I1673" s="4" t="s">
         <v>406</v>
@@ -62337,10 +62304,10 @@
         <v>1086</v>
       </c>
       <c r="B1674" s="8" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="C1674" s="9" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="D1674" s="10">
         <v>2</v>
@@ -62355,7 +62322,7 @@
         <v>16</v>
       </c>
       <c r="H1674" s="8" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="I1674" s="4" t="s">
         <v>101</v>
@@ -62384,7 +62351,7 @@
         <v>82</v>
       </c>
       <c r="H1675" s="1" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="I1675" s="4" t="s">
         <v>101</v>
@@ -62409,10 +62376,10 @@
         <v>30</v>
       </c>
       <c r="H1676" s="1" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="I1676" s="4" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="J1676" s="4" t="s">
         <v>37</v>
@@ -62432,7 +62399,7 @@
       <c r="F1677" s="13"/>
       <c r="G1677" s="13"/>
       <c r="H1677" s="1" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="I1677" s="13"/>
       <c r="J1677" s="13"/>
@@ -62449,7 +62416,7 @@
       <c r="F1678" s="13"/>
       <c r="G1678" s="13"/>
       <c r="H1678" s="1" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="I1678" s="13"/>
       <c r="J1678" s="13"/>
@@ -62466,7 +62433,7 @@
       <c r="F1679" s="13"/>
       <c r="G1679" s="13"/>
       <c r="H1679" s="1" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="I1679" s="13"/>
       <c r="J1679" s="13"/>
@@ -62485,10 +62452,10 @@
         <v>35</v>
       </c>
       <c r="H1680" s="1" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="I1680" s="4" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="J1680" s="4" t="s">
         <v>52</v>
@@ -62508,7 +62475,7 @@
       <c r="F1681" s="13"/>
       <c r="G1681" s="13"/>
       <c r="H1681" s="1" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="I1681" s="13"/>
       <c r="J1681" s="13"/>
@@ -62525,7 +62492,7 @@
       <c r="F1682" s="14"/>
       <c r="G1682" s="14"/>
       <c r="H1682" s="9" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="I1682" s="14"/>
       <c r="J1682" s="14"/>
@@ -62542,7 +62509,7 @@
       <c r="F1683" s="13"/>
       <c r="G1683" s="13"/>
       <c r="H1683" s="1" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="I1683" s="13"/>
       <c r="J1683" s="13"/>
@@ -62559,7 +62526,7 @@
       <c r="F1684" s="13"/>
       <c r="G1684" s="13"/>
       <c r="H1684" s="1" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="I1684" s="13"/>
       <c r="J1684" s="13"/>
@@ -62572,10 +62539,10 @@
         <v>1863</v>
       </c>
       <c r="B1685" s="8" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="C1685" s="9" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="D1685" s="10">
         <v>2</v>
@@ -62590,7 +62557,7 @@
         <v>16</v>
       </c>
       <c r="H1685" s="8" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="I1685" s="4" t="s">
         <v>101</v>
@@ -62617,7 +62584,7 @@
       <c r="F1686" s="13"/>
       <c r="G1686" s="13"/>
       <c r="H1686" s="1" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="I1686" s="13"/>
       <c r="J1686" s="13"/>
@@ -62636,7 +62603,7 @@
         <v>82</v>
       </c>
       <c r="H1687" s="1" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="I1687" s="4" t="s">
         <v>101</v>
@@ -62661,7 +62628,7 @@
         <v>91</v>
       </c>
       <c r="H1688" s="1" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="I1688" s="4" t="s">
         <v>103</v>
@@ -62686,10 +62653,10 @@
         <v>30</v>
       </c>
       <c r="H1689" s="1" t="s">
+        <v>1578</v>
+      </c>
+      <c r="I1689" s="4" t="s">
         <v>1580</v>
-      </c>
-      <c r="I1689" s="4" t="s">
-        <v>1582</v>
       </c>
       <c r="J1689" s="4" t="s">
         <v>33</v>
@@ -62709,7 +62676,7 @@
       <c r="F1690" s="13"/>
       <c r="G1690" s="13"/>
       <c r="H1690" s="1" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="I1690" s="13"/>
       <c r="J1690" s="13"/>
@@ -62726,7 +62693,7 @@
       <c r="F1691" s="13"/>
       <c r="G1691" s="13"/>
       <c r="H1691" s="1" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="I1691" s="13"/>
       <c r="J1691" s="13"/>
@@ -62743,7 +62710,7 @@
       <c r="F1692" s="13"/>
       <c r="G1692" s="13"/>
       <c r="H1692" s="1" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="I1692" s="13"/>
       <c r="J1692" s="13"/>
@@ -62762,10 +62729,10 @@
         <v>35</v>
       </c>
       <c r="H1693" s="1" t="s">
+        <v>1578</v>
+      </c>
+      <c r="I1693" s="4" t="s">
         <v>1580</v>
-      </c>
-      <c r="I1693" s="4" t="s">
-        <v>1582</v>
       </c>
       <c r="J1693" s="4" t="s">
         <v>48</v>
@@ -62785,7 +62752,7 @@
       <c r="F1694" s="13"/>
       <c r="G1694" s="13"/>
       <c r="H1694" s="1" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="I1694" s="13"/>
       <c r="J1694" s="13"/>
@@ -62802,7 +62769,7 @@
       <c r="F1695" s="13"/>
       <c r="G1695" s="13"/>
       <c r="H1695" s="1" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="I1695" s="13"/>
       <c r="J1695" s="13"/>
@@ -62815,10 +62782,10 @@
         <v>2505</v>
       </c>
       <c r="B1696" s="8" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="C1696" s="9" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="D1696" s="10">
         <v>2</v>
@@ -62833,7 +62800,7 @@
         <v>16</v>
       </c>
       <c r="H1696" s="8" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
       <c r="I1696" s="4" t="s">
         <v>101</v>
@@ -62862,7 +62829,7 @@
         <v>82</v>
       </c>
       <c r="H1697" s="1" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="I1697" s="4" t="s">
         <v>101</v>
@@ -62887,10 +62854,10 @@
         <v>30</v>
       </c>
       <c r="H1698" s="1" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="I1698" s="4" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="J1698" s="4" t="s">
         <v>48</v>
@@ -62910,7 +62877,7 @@
       <c r="F1699" s="13"/>
       <c r="G1699" s="13"/>
       <c r="H1699" s="1" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="I1699" s="13"/>
       <c r="J1699" s="13"/>
@@ -62927,7 +62894,7 @@
       <c r="F1700" s="13"/>
       <c r="G1700" s="13"/>
       <c r="H1700" s="1" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
       <c r="I1700" s="13"/>
       <c r="J1700" s="13"/>
@@ -62946,10 +62913,10 @@
         <v>35</v>
       </c>
       <c r="H1701" s="1" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="I1701" s="4" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="J1701" s="4" t="s">
         <v>33</v>
@@ -62969,7 +62936,7 @@
       <c r="F1702" s="13"/>
       <c r="G1702" s="13"/>
       <c r="H1702" s="1" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="I1702" s="13"/>
       <c r="J1702" s="13"/>
@@ -62986,7 +62953,7 @@
       <c r="F1703" s="13"/>
       <c r="G1703" s="13"/>
       <c r="H1703" s="1" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
       <c r="I1703" s="13"/>
       <c r="J1703" s="13"/>
@@ -62999,10 +62966,10 @@
         <v>1294</v>
       </c>
       <c r="B1704" s="8" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="C1704" s="8" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
       <c r="D1704" s="10">
         <v>2</v>
@@ -63017,7 +62984,7 @@
         <v>16</v>
       </c>
       <c r="H1704" s="9" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="I1704" s="4" t="s">
         <v>101</v>
@@ -63044,7 +63011,7 @@
       <c r="F1705" s="13"/>
       <c r="G1705" s="13"/>
       <c r="H1705" s="1" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="I1705" s="13"/>
       <c r="J1705" s="13"/>
@@ -63063,7 +63030,7 @@
         <v>82</v>
       </c>
       <c r="H1706" s="8" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="I1706" s="4" t="s">
         <v>101</v>
@@ -63086,7 +63053,7 @@
       <c r="F1707" s="13"/>
       <c r="G1707" s="13"/>
       <c r="H1707" s="1" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="I1707" s="13"/>
       <c r="J1707" s="13"/>
@@ -63105,10 +63072,10 @@
         <v>30</v>
       </c>
       <c r="H1708" s="8" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="I1708" s="4" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="J1708" s="4" t="s">
         <v>37</v>
@@ -63128,7 +63095,7 @@
       <c r="F1709" s="13"/>
       <c r="G1709" s="13"/>
       <c r="H1709" s="1" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="I1709" s="13"/>
       <c r="J1709" s="13"/>
@@ -63145,7 +63112,7 @@
       <c r="F1710" s="13"/>
       <c r="G1710" s="13"/>
       <c r="H1710" s="1" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
       <c r="I1710" s="13"/>
       <c r="J1710" s="13"/>
@@ -63162,7 +63129,7 @@
       <c r="F1711" s="13"/>
       <c r="G1711" s="13"/>
       <c r="H1711" s="1" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="I1711" s="13"/>
       <c r="J1711" s="13"/>
@@ -63179,7 +63146,7 @@
       <c r="F1712" s="13"/>
       <c r="G1712" s="13"/>
       <c r="H1712" s="1" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="I1712" s="13"/>
       <c r="J1712" s="13"/>
@@ -63198,10 +63165,10 @@
         <v>35</v>
       </c>
       <c r="H1713" s="8" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="I1713" s="4" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="J1713" s="4" t="s">
         <v>52</v>
@@ -63221,7 +63188,7 @@
       <c r="F1714" s="13"/>
       <c r="G1714" s="13"/>
       <c r="H1714" s="1" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="I1714" s="13"/>
       <c r="J1714" s="13"/>
@@ -63238,7 +63205,7 @@
       <c r="F1715" s="13"/>
       <c r="G1715" s="13"/>
       <c r="H1715" s="1" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
       <c r="I1715" s="13"/>
       <c r="J1715" s="13"/>
@@ -63255,7 +63222,7 @@
       <c r="F1716" s="13"/>
       <c r="G1716" s="13"/>
       <c r="H1716" s="1" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="I1716" s="13"/>
       <c r="J1716" s="13"/>
@@ -63272,7 +63239,7 @@
       <c r="F1717" s="13"/>
       <c r="G1717" s="13"/>
       <c r="H1717" s="1" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="I1717" s="13"/>
       <c r="J1717" s="13"/>
@@ -63289,7 +63256,7 @@
       <c r="F1718" s="13"/>
       <c r="G1718" s="13"/>
       <c r="H1718" s="1" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="I1718" s="13"/>
       <c r="J1718" s="13"/>
@@ -63302,7 +63269,7 @@
         <v>1665</v>
       </c>
       <c r="B1719" s="1" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="C1719" s="1" t="s">
         <v>466</v>
@@ -63318,7 +63285,7 @@
       </c>
       <c r="G1719" s="13"/>
       <c r="H1719" s="1" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="I1719" s="13"/>
       <c r="J1719" s="13"/>
@@ -63331,10 +63298,10 @@
         <v>1295</v>
       </c>
       <c r="B1720" s="1" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="C1720" s="1" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
       <c r="D1720" s="10">
         <v>2</v>
@@ -63349,7 +63316,7 @@
         <v>16</v>
       </c>
       <c r="H1720" s="1" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="I1720" s="4" t="s">
         <v>101</v>
@@ -63376,7 +63343,7 @@
       <c r="F1721" s="13"/>
       <c r="G1721" s="13"/>
       <c r="H1721" s="1" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="I1721" s="13"/>
       <c r="J1721" s="13"/>
@@ -63395,7 +63362,7 @@
         <v>82</v>
       </c>
       <c r="H1722" s="1" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="I1722" s="4" t="s">
         <v>161</v>
@@ -63418,7 +63385,7 @@
       <c r="F1723" s="13"/>
       <c r="G1723" s="13"/>
       <c r="H1723" s="1" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="I1723" s="13"/>
       <c r="J1723" s="13"/>
@@ -63437,10 +63404,10 @@
         <v>30</v>
       </c>
       <c r="H1724" s="1" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="I1724" s="4" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="J1724" s="4" t="s">
         <v>37</v>
@@ -63460,7 +63427,7 @@
       <c r="F1725" s="13"/>
       <c r="G1725" s="13"/>
       <c r="H1725" s="1" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
       <c r="I1725" s="13"/>
       <c r="J1725" s="13"/>
@@ -63477,7 +63444,7 @@
       <c r="F1726" s="13"/>
       <c r="G1726" s="13"/>
       <c r="H1726" s="1" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="I1726" s="13"/>
       <c r="J1726" s="13"/>
@@ -63494,7 +63461,7 @@
       <c r="F1727" s="13"/>
       <c r="G1727" s="13"/>
       <c r="H1727" s="1" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="I1727" s="13"/>
       <c r="J1727" s="13"/>
@@ -63511,7 +63478,7 @@
       <c r="F1728" s="13"/>
       <c r="G1728" s="13"/>
       <c r="H1728" s="1" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="I1728" s="13"/>
       <c r="J1728" s="13"/>
@@ -63530,10 +63497,10 @@
         <v>35</v>
       </c>
       <c r="H1729" s="1" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="I1729" s="4" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="J1729" s="4" t="s">
         <v>52</v>
@@ -63553,7 +63520,7 @@
       <c r="F1730" s="13"/>
       <c r="G1730" s="13"/>
       <c r="H1730" s="1" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
       <c r="I1730" s="13"/>
       <c r="J1730" s="13"/>
@@ -63570,7 +63537,7 @@
       <c r="F1731" s="13"/>
       <c r="G1731" s="13"/>
       <c r="H1731" s="1" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="I1731" s="13"/>
       <c r="J1731" s="13"/>
@@ -63587,7 +63554,7 @@
       <c r="F1732" s="13"/>
       <c r="G1732" s="13"/>
       <c r="H1732" s="1" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
       <c r="I1732" s="13"/>
       <c r="J1732" s="13"/>
@@ -63600,10 +63567,10 @@
         <v>1297</v>
       </c>
       <c r="B1733" s="1" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
       <c r="C1733" s="1" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="D1733" s="10">
         <v>2</v>
@@ -63618,7 +63585,7 @@
         <v>16</v>
       </c>
       <c r="H1733" s="1" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
       <c r="I1733" s="4" t="s">
         <v>101</v>
@@ -63645,7 +63612,7 @@
       <c r="F1734" s="13"/>
       <c r="G1734" s="13"/>
       <c r="H1734" s="1" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="I1734" s="13"/>
       <c r="J1734" s="13"/>
@@ -63664,7 +63631,7 @@
         <v>82</v>
       </c>
       <c r="H1735" s="1" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
       <c r="I1735" s="4" t="s">
         <v>101</v>
@@ -63687,7 +63654,7 @@
       <c r="F1736" s="13"/>
       <c r="G1736" s="13"/>
       <c r="H1736" s="1" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="I1736" s="13"/>
       <c r="J1736" s="13"/>
@@ -63706,10 +63673,10 @@
         <v>30</v>
       </c>
       <c r="H1737" s="1" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
       <c r="I1737" s="4" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="J1737" s="4" t="s">
         <v>33</v>
@@ -63729,7 +63696,7 @@
       <c r="F1738" s="13"/>
       <c r="G1738" s="13"/>
       <c r="H1738" s="1" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
       <c r="I1738" s="13"/>
       <c r="J1738" s="13"/>
@@ -63746,7 +63713,7 @@
       <c r="F1739" s="13"/>
       <c r="G1739" s="13"/>
       <c r="H1739" s="1" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
       <c r="I1739" s="13"/>
       <c r="J1739" s="13"/>
@@ -63763,7 +63730,7 @@
       <c r="F1740" s="13"/>
       <c r="G1740" s="13"/>
       <c r="H1740" s="1" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
       <c r="I1740" s="13"/>
       <c r="J1740" s="13"/>
@@ -63780,7 +63747,7 @@
       <c r="F1741" s="13"/>
       <c r="G1741" s="13"/>
       <c r="H1741" s="1" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="I1741" s="13"/>
       <c r="J1741" s="13"/>
@@ -63799,10 +63766,10 @@
         <v>35</v>
       </c>
       <c r="H1742" s="1" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
       <c r="I1742" s="4" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="J1742" s="4" t="s">
         <v>41</v>
@@ -63822,7 +63789,7 @@
       <c r="F1743" s="13"/>
       <c r="G1743" s="13"/>
       <c r="H1743" s="1" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="I1743" s="13"/>
       <c r="J1743" s="13"/>
@@ -63839,7 +63806,7 @@
       <c r="F1744" s="13"/>
       <c r="G1744" s="13"/>
       <c r="H1744" s="1" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="I1744" s="13"/>
       <c r="J1744" s="13"/>
@@ -63856,7 +63823,7 @@
       <c r="F1745" s="13"/>
       <c r="G1745" s="13"/>
       <c r="H1745" s="1" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="I1745" s="13"/>
       <c r="J1745" s="13"/>
@@ -63873,7 +63840,7 @@
       <c r="F1746" s="13"/>
       <c r="G1746" s="13"/>
       <c r="H1746" s="1" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
       <c r="I1746" s="13"/>
       <c r="J1746" s="13"/>
@@ -63886,10 +63853,10 @@
         <v>2506</v>
       </c>
       <c r="B1747" s="8" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="C1747" s="9" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="D1747" s="10">
         <v>2</v>
@@ -63904,7 +63871,7 @@
         <v>16</v>
       </c>
       <c r="H1747" s="8" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="I1747" s="4" t="s">
         <v>101</v>
@@ -63933,7 +63900,7 @@
         <v>82</v>
       </c>
       <c r="H1748" s="1" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="I1748" s="4" t="s">
         <v>101</v>
@@ -63958,10 +63925,10 @@
         <v>30</v>
       </c>
       <c r="H1749" s="1" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="I1749" s="4" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="J1749" s="4" t="s">
         <v>48</v>
@@ -63981,7 +63948,7 @@
       <c r="F1750" s="13"/>
       <c r="G1750" s="13"/>
       <c r="H1750" s="1" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
       <c r="I1750" s="13"/>
       <c r="J1750" s="13"/>
@@ -63998,7 +63965,7 @@
       <c r="F1751" s="13"/>
       <c r="G1751" s="13"/>
       <c r="H1751" s="1" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
       <c r="I1751" s="13"/>
       <c r="J1751" s="13"/>
@@ -64015,7 +63982,7 @@
       <c r="F1752" s="13"/>
       <c r="G1752" s="13"/>
       <c r="H1752" s="1" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="I1752" s="13"/>
       <c r="J1752" s="13"/>
@@ -64032,7 +63999,7 @@
       <c r="F1753" s="13"/>
       <c r="G1753" s="13"/>
       <c r="H1753" s="1" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="I1753" s="13"/>
       <c r="J1753" s="13"/>
@@ -64051,10 +64018,10 @@
         <v>35</v>
       </c>
       <c r="H1754" s="1" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="I1754" s="4" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="J1754" s="4" t="s">
         <v>41</v>
@@ -64074,7 +64041,7 @@
       <c r="F1755" s="14"/>
       <c r="G1755" s="14"/>
       <c r="H1755" s="9" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
       <c r="I1755" s="14"/>
       <c r="J1755" s="14"/>
@@ -64091,7 +64058,7 @@
       <c r="F1756" s="13"/>
       <c r="G1756" s="13"/>
       <c r="H1756" s="1" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
       <c r="I1756" s="13"/>
       <c r="J1756" s="13"/>
@@ -64104,7 +64071,7 @@
         <v>1682</v>
       </c>
       <c r="B1757" s="1" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
       <c r="C1757" s="1" t="s">
         <v>491</v>
@@ -64120,7 +64087,7 @@
       </c>
       <c r="G1757" s="13"/>
       <c r="H1757" s="1" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="I1757" s="13"/>
       <c r="J1757" s="13"/>
@@ -64133,7 +64100,7 @@
         <v>1750</v>
       </c>
       <c r="B1758" s="1" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
       <c r="C1758" s="1" t="s">
         <v>491</v>
@@ -64149,7 +64116,7 @@
       </c>
       <c r="G1758" s="13"/>
       <c r="H1758" s="1" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="I1758" s="13"/>
       <c r="J1758" s="13"/>
@@ -64162,7 +64129,7 @@
         <v>1699</v>
       </c>
       <c r="B1759" s="1" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
       <c r="C1759" s="1" t="s">
         <v>494</v>
@@ -64178,7 +64145,7 @@
       </c>
       <c r="G1759" s="13"/>
       <c r="H1759" s="1" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="I1759" s="13"/>
       <c r="J1759" s="13"/>
@@ -64191,7 +64158,7 @@
         <v>1766</v>
       </c>
       <c r="B1760" s="1" t="s">
-        <v>1647</v>
+        <v>1645</v>
       </c>
       <c r="C1760" s="1" t="s">
         <v>494</v>
@@ -64207,7 +64174,7 @@
       </c>
       <c r="G1760" s="13"/>
       <c r="H1760" s="1" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="I1760" s="13"/>
       <c r="J1760" s="13"/>
@@ -64220,10 +64187,10 @@
         <v>1305</v>
       </c>
       <c r="B1761" s="1" t="s">
-        <v>1648</v>
+        <v>1646</v>
       </c>
       <c r="C1761" s="1" t="s">
-        <v>1649</v>
+        <v>1647</v>
       </c>
       <c r="D1761" s="10">
         <v>3</v>
@@ -64238,7 +64205,7 @@
         <v>16</v>
       </c>
       <c r="H1761" s="1" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
       <c r="I1761" s="4" t="s">
         <v>261</v>
@@ -64261,10 +64228,10 @@
         <v>1308</v>
       </c>
       <c r="B1762" s="1" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="C1762" s="1" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
       <c r="D1762" s="10">
         <v>2</v>
@@ -64279,7 +64246,7 @@
         <v>16</v>
       </c>
       <c r="H1762" s="1" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="I1762" s="4" t="s">
         <v>261</v>
@@ -64308,10 +64275,10 @@
         <v>30</v>
       </c>
       <c r="H1763" s="1" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="I1763" s="4" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="J1763" s="4" t="s">
         <v>41</v>
@@ -64331,7 +64298,7 @@
       <c r="F1764" s="13"/>
       <c r="G1764" s="13"/>
       <c r="H1764" s="1" t="s">
-        <v>1655</v>
+        <v>1653</v>
       </c>
       <c r="I1764" s="13"/>
       <c r="J1764" s="13"/>
@@ -64348,7 +64315,7 @@
       <c r="F1765" s="13"/>
       <c r="G1765" s="13"/>
       <c r="H1765" s="1" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
       <c r="I1765" s="13"/>
       <c r="J1765" s="13"/>
@@ -64365,7 +64332,7 @@
       <c r="F1766" s="13"/>
       <c r="G1766" s="13"/>
       <c r="H1766" s="1" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="I1766" s="13"/>
       <c r="J1766" s="13"/>
@@ -64382,7 +64349,7 @@
       <c r="F1767" s="13"/>
       <c r="G1767" s="13"/>
       <c r="H1767" s="1" t="s">
-        <v>1658</v>
+        <v>1656</v>
       </c>
       <c r="I1767" s="13"/>
       <c r="J1767" s="13"/>
@@ -64395,10 +64362,10 @@
         <v>2382</v>
       </c>
       <c r="B1768" s="1" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
       <c r="C1768" s="1" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
       <c r="D1768" s="10">
         <v>3</v>
@@ -64413,7 +64380,7 @@
         <v>16</v>
       </c>
       <c r="H1768" s="1" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="I1768" s="4" t="s">
         <v>161</v>
@@ -64440,7 +64407,7 @@
       <c r="F1769" s="13"/>
       <c r="G1769" s="13"/>
       <c r="H1769" s="1" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
       <c r="I1769" s="13"/>
       <c r="J1769" s="13"/>
@@ -64453,10 +64420,10 @@
         <v>2384</v>
       </c>
       <c r="B1770" s="8" t="s">
-        <v>1662</v>
+        <v>1660</v>
       </c>
       <c r="C1770" s="9" t="s">
-        <v>1663</v>
+        <v>1661</v>
       </c>
       <c r="D1770" s="10">
         <v>3</v>
@@ -64471,7 +64438,7 @@
         <v>16</v>
       </c>
       <c r="H1770" s="8" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
       <c r="I1770" s="4" t="s">
         <v>161</v>
@@ -64494,10 +64461,10 @@
         <v>2385</v>
       </c>
       <c r="B1771" s="8" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="C1771" s="8" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
       <c r="D1771" s="10">
         <v>3</v>
@@ -64512,7 +64479,7 @@
         <v>16</v>
       </c>
       <c r="H1771" s="8" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="I1771" s="4" t="s">
         <v>96</v>
@@ -64539,7 +64506,7 @@
       <c r="F1772" s="13"/>
       <c r="G1772" s="13"/>
       <c r="H1772" s="1" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="I1772" s="4" t="s">
         <v>96</v>
@@ -64554,14 +64521,14 @@
       <c r="M1772" s="13"/>
     </row>
     <row r="1773" spans="1:13" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1773" s="19">
+      <c r="A1773" s="18">
         <v>2387</v>
       </c>
-      <c r="B1773" s="20" t="s">
-        <v>1667</v>
+      <c r="B1773" s="19" t="s">
+        <v>1665</v>
       </c>
       <c r="C1773" s="1" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="D1773" s="10">
         <v>3</v>
@@ -64572,11 +64539,11 @@
       <c r="F1773" s="10">
         <v>4</v>
       </c>
-      <c r="G1773" s="21" t="s">
+      <c r="G1773" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H1773" s="20" t="s">
-        <v>1669</v>
+      <c r="H1773" s="19" t="s">
+        <v>1667</v>
       </c>
       <c r="I1773" s="4" t="s">
         <v>161</v>
@@ -64605,7 +64572,7 @@
         <v>30</v>
       </c>
       <c r="H1774" s="1" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
       <c r="I1774" s="4" t="s">
         <v>723</v>
@@ -64628,7 +64595,7 @@
       <c r="F1775" s="14"/>
       <c r="G1775" s="14"/>
       <c r="H1775" s="9" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
       <c r="I1775" s="14"/>
       <c r="J1775" s="14"/>
@@ -64645,7 +64612,7 @@
       <c r="F1776" s="13"/>
       <c r="G1776" s="13"/>
       <c r="H1776" s="1" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
       <c r="I1776" s="13"/>
       <c r="J1776" s="13"/>
@@ -64662,7 +64629,7 @@
       <c r="F1777" s="13"/>
       <c r="G1777" s="13"/>
       <c r="H1777" s="1" t="s">
-        <v>1673</v>
+        <v>1671</v>
       </c>
       <c r="I1777" s="13"/>
       <c r="J1777" s="13"/>
@@ -64679,7 +64646,7 @@
       <c r="F1778" s="13"/>
       <c r="G1778" s="13"/>
       <c r="H1778" s="1" t="s">
-        <v>1674</v>
+        <v>1672</v>
       </c>
       <c r="I1778" s="13"/>
       <c r="J1778" s="13"/>
@@ -64696,7 +64663,7 @@
       <c r="F1779" s="13"/>
       <c r="G1779" s="13"/>
       <c r="H1779" s="1" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
       <c r="I1779" s="13"/>
       <c r="J1779" s="13"/>
@@ -64713,7 +64680,7 @@
       <c r="F1780" s="13"/>
       <c r="G1780" s="13"/>
       <c r="H1780" s="1" t="s">
-        <v>1676</v>
+        <v>1674</v>
       </c>
       <c r="I1780" s="13"/>
       <c r="J1780" s="13"/>
@@ -64730,7 +64697,7 @@
       <c r="F1781" s="13"/>
       <c r="G1781" s="13"/>
       <c r="H1781" s="1" t="s">
-        <v>1677</v>
+        <v>1675</v>
       </c>
       <c r="I1781" s="13"/>
       <c r="J1781" s="13"/>
@@ -64743,10 +64710,10 @@
         <v>653</v>
       </c>
       <c r="B1782" s="8" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
       <c r="C1782" s="9" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="D1782" s="10">
         <v>3</v>
@@ -64761,7 +64728,7 @@
         <v>16</v>
       </c>
       <c r="H1782" s="9" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="I1782" s="4" t="s">
         <v>161</v>
@@ -64788,7 +64755,7 @@
       <c r="F1783" s="14"/>
       <c r="G1783" s="14"/>
       <c r="H1783" s="8" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="I1783" s="4" t="s">
         <v>161</v>
@@ -64813,10 +64780,10 @@
         <v>30</v>
       </c>
       <c r="H1784" s="8" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="I1784" s="4" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="J1784" s="4" t="s">
         <v>210</v>
@@ -64836,7 +64803,7 @@
       <c r="F1785" s="13"/>
       <c r="G1785" s="13"/>
       <c r="H1785" s="1" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
       <c r="I1785" s="13"/>
       <c r="J1785" s="13"/>
@@ -64853,7 +64820,7 @@
       <c r="F1786" s="13"/>
       <c r="G1786" s="13"/>
       <c r="H1786" s="1" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="I1786" s="13"/>
       <c r="J1786" s="13"/>
@@ -64870,7 +64837,7 @@
       <c r="F1787" s="13"/>
       <c r="G1787" s="13"/>
       <c r="H1787" s="1" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
       <c r="I1787" s="13"/>
       <c r="J1787" s="13"/>
@@ -64883,10 +64850,10 @@
         <v>55</v>
       </c>
       <c r="B1788" s="1" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="C1788" s="1" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="D1788" s="10">
         <v>3</v>
@@ -64901,7 +64868,7 @@
         <v>16</v>
       </c>
       <c r="H1788" s="1" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
       <c r="I1788" s="4" t="s">
         <v>167</v>
@@ -64928,7 +64895,7 @@
       <c r="F1789" s="13"/>
       <c r="G1789" s="13"/>
       <c r="H1789" s="1" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="I1789" s="4" t="s">
         <v>167</v>
@@ -64947,10 +64914,10 @@
         <v>2132</v>
       </c>
       <c r="B1790" s="8" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
       <c r="C1790" s="9" t="s">
-        <v>1687</v>
+        <v>1685</v>
       </c>
       <c r="D1790" s="10">
         <v>3</v>
@@ -64965,7 +64932,7 @@
         <v>16</v>
       </c>
       <c r="H1790" s="8" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
       <c r="I1790" s="4" t="s">
         <v>106</v>
@@ -64992,7 +64959,7 @@
       <c r="F1791" s="13"/>
       <c r="G1791" s="13"/>
       <c r="H1791" s="1" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
       <c r="I1791" s="13"/>
       <c r="J1791" s="13"/>
@@ -65005,10 +64972,10 @@
         <v>2293</v>
       </c>
       <c r="B1792" s="8" t="s">
-        <v>1689</v>
+        <v>1687</v>
       </c>
       <c r="C1792" s="9" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
       <c r="D1792" s="10">
         <v>3</v>
@@ -65023,7 +64990,7 @@
         <v>16</v>
       </c>
       <c r="H1792" s="8" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="I1792" s="4" t="s">
         <v>96</v>
@@ -65052,16 +65019,16 @@
         <v>30</v>
       </c>
       <c r="H1793" s="1" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
       <c r="I1793" s="4" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="J1793" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K1793" s="4" t="s">
-        <v>1693</v>
+      <c r="K1793" s="4">
+        <v>6789</v>
       </c>
       <c r="L1793" s="13"/>
       <c r="M1793" s="13"/>
@@ -65075,7 +65042,7 @@
       <c r="F1794" s="13"/>
       <c r="G1794" s="13"/>
       <c r="H1794" s="1" t="s">
-        <v>1694</v>
+        <v>1691</v>
       </c>
       <c r="I1794" s="13"/>
       <c r="J1794" s="13"/>
@@ -65088,10 +65055,10 @@
         <v>2105</v>
       </c>
       <c r="B1795" s="8" t="s">
-        <v>1695</v>
+        <v>1692</v>
       </c>
       <c r="C1795" s="9" t="s">
-        <v>1696</v>
+        <v>1693</v>
       </c>
       <c r="D1795" s="10">
         <v>3</v>
@@ -65106,7 +65073,7 @@
         <v>16</v>
       </c>
       <c r="H1795" s="8" t="s">
-        <v>1697</v>
+        <v>1694</v>
       </c>
       <c r="I1795" s="4" t="s">
         <v>25</v>
@@ -65135,10 +65102,10 @@
         <v>30</v>
       </c>
       <c r="H1796" s="1" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="I1796" s="4" t="s">
-        <v>1699</v>
+        <v>1696</v>
       </c>
       <c r="J1796" s="4" t="s">
         <v>119</v>
@@ -65158,7 +65125,7 @@
       <c r="F1797" s="13"/>
       <c r="G1797" s="13"/>
       <c r="H1797" s="1" t="s">
-        <v>1700</v>
+        <v>1697</v>
       </c>
       <c r="I1797" s="13"/>
       <c r="J1797" s="13"/>
@@ -65175,7 +65142,7 @@
       <c r="F1798" s="13"/>
       <c r="G1798" s="13"/>
       <c r="H1798" s="1" t="s">
-        <v>1701</v>
+        <v>1698</v>
       </c>
       <c r="I1798" s="13"/>
       <c r="J1798" s="13"/>
@@ -65192,7 +65159,7 @@
       <c r="F1799" s="14"/>
       <c r="G1799" s="14"/>
       <c r="H1799" s="8" t="s">
-        <v>1702</v>
+        <v>1699</v>
       </c>
       <c r="I1799" s="14"/>
       <c r="J1799" s="14"/>
@@ -65205,10 +65172,10 @@
         <v>2391</v>
       </c>
       <c r="B1800" s="8" t="s">
-        <v>1703</v>
+        <v>1700</v>
       </c>
       <c r="C1800" s="9" t="s">
-        <v>1704</v>
+        <v>1701</v>
       </c>
       <c r="D1800" s="10">
         <v>3</v>
@@ -65223,7 +65190,7 @@
         <v>16</v>
       </c>
       <c r="H1800" s="8" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
       <c r="I1800" s="4" t="s">
         <v>96</v>
@@ -65246,10 +65213,10 @@
         <v>2392</v>
       </c>
       <c r="B1801" s="1" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="C1801" s="1" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="D1801" s="10">
         <v>3</v>
@@ -65264,7 +65231,7 @@
         <v>16</v>
       </c>
       <c r="H1801" s="1" t="s">
-        <v>1707</v>
+        <v>1704</v>
       </c>
       <c r="I1801" s="4" t="s">
         <v>161</v>
@@ -65291,7 +65258,7 @@
       <c r="F1802" s="13"/>
       <c r="G1802" s="13"/>
       <c r="H1802" s="1" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="I1802" s="4" t="s">
         <v>161</v>
@@ -65310,10 +65277,10 @@
         <v>721</v>
       </c>
       <c r="B1803" s="1" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="C1803" s="1" t="s">
-        <v>1709</v>
+        <v>1706</v>
       </c>
       <c r="D1803" s="10">
         <v>3</v>
@@ -65328,7 +65295,7 @@
         <v>16</v>
       </c>
       <c r="H1803" s="1" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="I1803" s="4" t="s">
         <v>161</v>
@@ -65355,7 +65322,7 @@
       <c r="F1804" s="13"/>
       <c r="G1804" s="13"/>
       <c r="H1804" s="1" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
       <c r="I1804" s="13"/>
       <c r="J1804" s="4" t="s">
@@ -65378,10 +65345,10 @@
         <v>30</v>
       </c>
       <c r="H1805" s="1" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
       <c r="I1805" s="4" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="J1805" s="4" t="s">
         <v>119</v>
@@ -65401,7 +65368,7 @@
       <c r="F1806" s="13"/>
       <c r="G1806" s="13"/>
       <c r="H1806" s="1" t="s">
-        <v>1710</v>
+        <v>1707</v>
       </c>
       <c r="I1806" s="13"/>
       <c r="J1806" s="13"/>
@@ -65418,7 +65385,7 @@
       <c r="F1807" s="13"/>
       <c r="G1807" s="13"/>
       <c r="H1807" s="1" t="s">
-        <v>1711</v>
+        <v>1708</v>
       </c>
       <c r="I1807" s="13"/>
       <c r="J1807" s="13"/>
@@ -65431,10 +65398,10 @@
         <v>1014</v>
       </c>
       <c r="B1808" s="1" t="s">
-        <v>1712</v>
+        <v>1709</v>
       </c>
       <c r="C1808" s="1" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
       <c r="D1808" s="10">
         <v>0</v>
@@ -65449,10 +65416,10 @@
         <v>30</v>
       </c>
       <c r="H1808" s="1" t="s">
-        <v>1714</v>
+        <v>1711</v>
       </c>
       <c r="I1808" s="4" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="J1808" s="4" t="s">
         <v>33</v>
@@ -65472,7 +65439,7 @@
       <c r="F1809" s="13"/>
       <c r="G1809" s="13"/>
       <c r="H1809" s="1" t="s">
-        <v>1716</v>
+        <v>1713</v>
       </c>
       <c r="I1809" s="13"/>
       <c r="J1809" s="13"/>
@@ -65491,10 +65458,10 @@
         <v>35</v>
       </c>
       <c r="H1810" s="1" t="s">
-        <v>1717</v>
+        <v>1714</v>
       </c>
       <c r="I1810" s="4" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="J1810" s="4" t="s">
         <v>48</v>
@@ -65514,7 +65481,7 @@
       <c r="F1811" s="13"/>
       <c r="G1811" s="13"/>
       <c r="H1811" s="1" t="s">
-        <v>1718</v>
+        <v>1715</v>
       </c>
       <c r="I1811" s="13"/>
       <c r="J1811" s="13"/>
@@ -65536,7 +65503,7 @@
         <v>939</v>
       </c>
       <c r="I1812" s="4" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="J1812" s="4" t="s">
         <v>41</v>
@@ -65556,7 +65523,7 @@
       <c r="F1813" s="13"/>
       <c r="G1813" s="13"/>
       <c r="H1813" s="1" t="s">
-        <v>1719</v>
+        <v>1716</v>
       </c>
       <c r="I1813" s="13"/>
       <c r="J1813" s="13"/>
@@ -65578,7 +65545,7 @@
         <v>936</v>
       </c>
       <c r="I1814" s="4" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="J1814" s="4" t="s">
         <v>37</v>
@@ -65598,7 +65565,7 @@
       <c r="F1815" s="13"/>
       <c r="G1815" s="13"/>
       <c r="H1815" s="1" t="s">
-        <v>1720</v>
+        <v>1717</v>
       </c>
       <c r="I1815" s="13"/>
       <c r="J1815" s="13"/>
@@ -65617,10 +65584,10 @@
         <v>46</v>
       </c>
       <c r="H1816" s="1" t="s">
-        <v>1721</v>
+        <v>1718</v>
       </c>
       <c r="I1816" s="4" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="J1816" s="4" t="s">
         <v>52</v>
@@ -65640,7 +65607,7 @@
       <c r="F1817" s="13"/>
       <c r="G1817" s="13"/>
       <c r="H1817" s="1" t="s">
-        <v>1722</v>
+        <v>1719</v>
       </c>
       <c r="I1817" s="13"/>
       <c r="J1817" s="13"/>
@@ -65662,7 +65629,7 @@
         <v>937</v>
       </c>
       <c r="I1818" s="4" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="J1818" s="4" t="s">
         <v>52</v>
@@ -65682,7 +65649,7 @@
       <c r="F1819" s="13"/>
       <c r="G1819" s="13"/>
       <c r="H1819" s="1" t="s">
-        <v>1723</v>
+        <v>1720</v>
       </c>
       <c r="I1819" s="13"/>
       <c r="J1819" s="13"/>
@@ -65701,10 +65668,10 @@
         <v>54</v>
       </c>
       <c r="H1820" s="1" t="s">
-        <v>1724</v>
+        <v>1721</v>
       </c>
       <c r="I1820" s="4" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="J1820" s="4" t="s">
         <v>48</v>
@@ -65724,7 +65691,7 @@
       <c r="F1821" s="13"/>
       <c r="G1821" s="13"/>
       <c r="H1821" s="1" t="s">
-        <v>1725</v>
+        <v>1722</v>
       </c>
       <c r="I1821" s="13"/>
       <c r="J1821" s="13"/>
@@ -65743,10 +65710,10 @@
         <v>57</v>
       </c>
       <c r="H1822" s="1" t="s">
-        <v>1726</v>
+        <v>1723</v>
       </c>
       <c r="I1822" s="4" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="J1822" s="4" t="s">
         <v>41</v>
@@ -65766,7 +65733,7 @@
       <c r="F1823" s="13"/>
       <c r="G1823" s="13"/>
       <c r="H1823" s="1" t="s">
-        <v>1727</v>
+        <v>1724</v>
       </c>
       <c r="I1823" s="13"/>
       <c r="J1823" s="13"/>
@@ -65788,7 +65755,7 @@
         <v>933</v>
       </c>
       <c r="I1824" s="4" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="J1824" s="4" t="s">
         <v>33</v>
@@ -65808,7 +65775,7 @@
       <c r="F1825" s="13"/>
       <c r="G1825" s="13"/>
       <c r="H1825" s="1" t="s">
-        <v>1728</v>
+        <v>1725</v>
       </c>
       <c r="I1825" s="13"/>
       <c r="J1825" s="13"/>
@@ -65827,10 +65794,10 @@
         <v>63</v>
       </c>
       <c r="H1826" s="9" t="s">
-        <v>1729</v>
+        <v>1726</v>
       </c>
       <c r="I1826" s="4" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="J1826" s="4" t="s">
         <v>52</v>
@@ -65850,7 +65817,7 @@
       <c r="F1827" s="13"/>
       <c r="G1827" s="13"/>
       <c r="H1827" s="1" t="s">
-        <v>1730</v>
+        <v>1727</v>
       </c>
       <c r="I1827" s="13"/>
       <c r="J1827" s="13"/>
@@ -65863,10 +65830,10 @@
         <v>1015</v>
       </c>
       <c r="B1828" s="1" t="s">
-        <v>1731</v>
+        <v>1728</v>
       </c>
       <c r="C1828" s="1" t="s">
-        <v>1732</v>
+        <v>1729</v>
       </c>
       <c r="D1828" s="10">
         <v>3</v>
@@ -65881,7 +65848,7 @@
         <v>16</v>
       </c>
       <c r="H1828" s="1" t="s">
-        <v>1721</v>
+        <v>1718</v>
       </c>
       <c r="I1828" s="4" t="s">
         <v>683</v>
@@ -65908,7 +65875,7 @@
       <c r="F1829" s="13"/>
       <c r="G1829" s="13"/>
       <c r="H1829" s="1" t="s">
-        <v>1733</v>
+        <v>1730</v>
       </c>
       <c r="I1829" s="13"/>
       <c r="J1829" s="13"/>
@@ -65925,7 +65892,7 @@
       <c r="F1830" s="13"/>
       <c r="G1830" s="13"/>
       <c r="H1830" s="1" t="s">
-        <v>1721</v>
+        <v>1718</v>
       </c>
       <c r="I1830" s="4" t="s">
         <v>683</v>
@@ -65948,7 +65915,7 @@
       <c r="F1831" s="13"/>
       <c r="G1831" s="13"/>
       <c r="H1831" s="1" t="s">
-        <v>1733</v>
+        <v>1730</v>
       </c>
       <c r="I1831" s="13"/>
       <c r="J1831" s="13"/>
@@ -65967,7 +65934,7 @@
         <v>78</v>
       </c>
       <c r="H1832" s="1" t="s">
-        <v>1721</v>
+        <v>1718</v>
       </c>
       <c r="I1832" s="4" t="s">
         <v>680</v>
@@ -65994,7 +65961,7 @@
       <c r="F1833" s="13"/>
       <c r="G1833" s="13"/>
       <c r="H1833" s="1" t="s">
-        <v>1733</v>
+        <v>1730</v>
       </c>
       <c r="I1833" s="13"/>
       <c r="J1833" s="13"/>
@@ -66063,7 +66030,7 @@
         <v>94</v>
       </c>
       <c r="H1836" s="1" t="s">
-        <v>1734</v>
+        <v>1731</v>
       </c>
       <c r="I1836" s="4" t="s">
         <v>787</v>
@@ -66088,7 +66055,7 @@
         <v>97</v>
       </c>
       <c r="H1837" s="1" t="s">
-        <v>1734</v>
+        <v>1731</v>
       </c>
       <c r="I1837" s="4" t="s">
         <v>96</v>
@@ -66113,7 +66080,7 @@
         <v>100</v>
       </c>
       <c r="H1838" s="1" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="I1838" s="4" t="s">
         <v>93</v>
@@ -66138,7 +66105,7 @@
         <v>102</v>
       </c>
       <c r="H1839" s="1" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="I1839" s="4" t="s">
         <v>93</v>
@@ -66163,7 +66130,7 @@
         <v>104</v>
       </c>
       <c r="H1840" s="1" t="s">
-        <v>1726</v>
+        <v>1723</v>
       </c>
       <c r="I1840" s="4" t="s">
         <v>537</v>
@@ -66188,7 +66155,7 @@
         <v>107</v>
       </c>
       <c r="H1841" s="1" t="s">
-        <v>1726</v>
+        <v>1723</v>
       </c>
       <c r="I1841" s="4" t="s">
         <v>537</v>
@@ -66238,7 +66205,7 @@
         <v>111</v>
       </c>
       <c r="H1843" s="1" t="s">
-        <v>1736</v>
+        <v>1733</v>
       </c>
       <c r="I1843" s="4" t="s">
         <v>116</v>
@@ -66257,10 +66224,10 @@
         <v>1859</v>
       </c>
       <c r="B1844" s="1" t="s">
-        <v>1737</v>
+        <v>1734</v>
       </c>
       <c r="C1844" s="1" t="s">
-        <v>1738</v>
+        <v>1735</v>
       </c>
       <c r="D1844" s="10">
         <v>3</v>
@@ -66275,7 +66242,7 @@
         <v>16</v>
       </c>
       <c r="H1844" s="1" t="s">
-        <v>1739</v>
+        <v>1736</v>
       </c>
       <c r="I1844" s="4" t="s">
         <v>537</v>
@@ -66302,7 +66269,7 @@
       <c r="F1845" s="13"/>
       <c r="G1845" s="13"/>
       <c r="H1845" s="1" t="s">
-        <v>1740</v>
+        <v>1737</v>
       </c>
       <c r="I1845" s="4" t="s">
         <v>537</v>
@@ -66327,7 +66294,7 @@
         <v>82</v>
       </c>
       <c r="H1846" s="8" t="s">
-        <v>1741</v>
+        <v>1738</v>
       </c>
       <c r="I1846" s="4" t="s">
         <v>618</v>
@@ -66346,10 +66313,10 @@
         <v>1126</v>
       </c>
       <c r="B1847" s="8" t="s">
-        <v>1742</v>
+        <v>1739</v>
       </c>
       <c r="C1847" s="8" t="s">
-        <v>1743</v>
+        <v>1740</v>
       </c>
       <c r="D1847" s="10">
         <v>3</v>
@@ -66364,7 +66331,7 @@
         <v>16</v>
       </c>
       <c r="H1847" s="9" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
       <c r="I1847" s="4" t="s">
         <v>261</v>
@@ -66435,7 +66402,7 @@
         <v>1127</v>
       </c>
       <c r="B1850" s="8" t="s">
-        <v>1745</v>
+        <v>1742</v>
       </c>
       <c r="C1850" s="8" t="s">
         <v>931</v>
@@ -66986,10 +66953,10 @@
         <v>1128</v>
       </c>
       <c r="B1871" s="1" t="s">
-        <v>1746</v>
+        <v>1743</v>
       </c>
       <c r="C1871" s="1" t="s">
-        <v>1747</v>
+        <v>1744</v>
       </c>
       <c r="D1871" s="10">
         <v>3</v>
@@ -67004,7 +66971,7 @@
         <v>16</v>
       </c>
       <c r="H1871" s="1" t="s">
-        <v>1748</v>
+        <v>1745</v>
       </c>
       <c r="I1871" s="4" t="s">
         <v>261</v>
@@ -67033,7 +67000,7 @@
         <v>82</v>
       </c>
       <c r="H1872" s="1" t="s">
-        <v>1733</v>
+        <v>1730</v>
       </c>
       <c r="I1872" s="4" t="s">
         <v>261</v>
@@ -67052,10 +67019,10 @@
         <v>1129</v>
       </c>
       <c r="B1873" s="8" t="s">
-        <v>1749</v>
+        <v>1746</v>
       </c>
       <c r="C1873" s="9" t="s">
-        <v>1750</v>
+        <v>1747</v>
       </c>
       <c r="D1873" s="10">
         <v>0</v>
@@ -67070,10 +67037,10 @@
         <v>30</v>
       </c>
       <c r="H1873" s="8" t="s">
-        <v>1751</v>
+        <v>1748</v>
       </c>
       <c r="I1873" s="4" t="s">
-        <v>1752</v>
+        <v>1749</v>
       </c>
       <c r="J1873" s="4" t="s">
         <v>194</v>
@@ -67093,7 +67060,7 @@
       <c r="F1874" s="13"/>
       <c r="G1874" s="13"/>
       <c r="H1874" s="1" t="s">
-        <v>1753</v>
+        <v>1750</v>
       </c>
       <c r="I1874" s="13"/>
       <c r="J1874" s="13"/>
@@ -67110,7 +67077,7 @@
       <c r="F1875" s="14"/>
       <c r="G1875" s="14"/>
       <c r="H1875" s="9" t="s">
-        <v>1754</v>
+        <v>1751</v>
       </c>
       <c r="I1875" s="14"/>
       <c r="J1875" s="14"/>
@@ -67129,10 +67096,10 @@
         <v>35</v>
       </c>
       <c r="H1876" s="1" t="s">
-        <v>1755</v>
+        <v>1752</v>
       </c>
       <c r="I1876" s="4" t="s">
-        <v>1752</v>
+        <v>1749</v>
       </c>
       <c r="J1876" s="4" t="s">
         <v>119</v>
@@ -67152,7 +67119,7 @@
       <c r="F1877" s="13"/>
       <c r="G1877" s="13"/>
       <c r="H1877" s="1" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="I1877" s="13"/>
       <c r="J1877" s="13"/>
@@ -67169,7 +67136,7 @@
       <c r="F1878" s="13"/>
       <c r="G1878" s="13"/>
       <c r="H1878" s="1" t="s">
-        <v>1756</v>
+        <v>1753</v>
       </c>
       <c r="I1878" s="13"/>
       <c r="J1878" s="13"/>
@@ -67182,7 +67149,7 @@
         <v>1666</v>
       </c>
       <c r="B1879" s="1" t="s">
-        <v>1757</v>
+        <v>1754</v>
       </c>
       <c r="C1879" s="1" t="s">
         <v>466</v>
@@ -67198,7 +67165,7 @@
       </c>
       <c r="G1879" s="13"/>
       <c r="H1879" s="1" t="s">
-        <v>1726</v>
+        <v>1723</v>
       </c>
       <c r="I1879" s="13"/>
       <c r="J1879" s="13"/>
@@ -67211,10 +67178,10 @@
         <v>1486</v>
       </c>
       <c r="B1880" s="8" t="s">
-        <v>1758</v>
+        <v>1755</v>
       </c>
       <c r="C1880" s="8" t="s">
-        <v>1759</v>
+        <v>1756</v>
       </c>
       <c r="D1880" s="10">
         <v>3</v>
@@ -67229,7 +67196,7 @@
         <v>16</v>
       </c>
       <c r="H1880" s="8" t="s">
-        <v>1739</v>
+        <v>1736</v>
       </c>
       <c r="I1880" s="4" t="s">
         <v>261</v>
@@ -67258,7 +67225,7 @@
         <v>82</v>
       </c>
       <c r="H1881" s="1" t="s">
-        <v>1740</v>
+        <v>1737</v>
       </c>
       <c r="I1881" s="4" t="s">
         <v>261</v>
@@ -67281,7 +67248,7 @@
       <c r="F1882" s="13"/>
       <c r="G1882" s="13"/>
       <c r="H1882" s="1" t="s">
-        <v>1760</v>
+        <v>1757</v>
       </c>
       <c r="I1882" s="13"/>
       <c r="J1882" s="13"/>
@@ -67294,10 +67261,10 @@
         <v>1487</v>
       </c>
       <c r="B1883" s="8" t="s">
-        <v>1761</v>
+        <v>1758</v>
       </c>
       <c r="C1883" s="8" t="s">
-        <v>1762</v>
+        <v>1759</v>
       </c>
       <c r="D1883" s="10">
         <v>3</v>
@@ -67312,7 +67279,7 @@
         <v>16</v>
       </c>
       <c r="H1883" s="8" t="s">
-        <v>1763</v>
+        <v>1760</v>
       </c>
       <c r="I1883" s="4" t="s">
         <v>261</v>
@@ -67341,7 +67308,7 @@
         <v>82</v>
       </c>
       <c r="H1884" s="1" t="s">
-        <v>1717</v>
+        <v>1714</v>
       </c>
       <c r="I1884" s="4" t="s">
         <v>261</v>
@@ -67364,7 +67331,7 @@
       <c r="F1885" s="13"/>
       <c r="G1885" s="13"/>
       <c r="H1885" s="1" t="s">
-        <v>1764</v>
+        <v>1761</v>
       </c>
       <c r="I1885" s="13"/>
       <c r="J1885" s="13"/>
@@ -67377,10 +67344,10 @@
         <v>1488</v>
       </c>
       <c r="B1886" s="8" t="s">
-        <v>1765</v>
+        <v>1762</v>
       </c>
       <c r="C1886" s="8" t="s">
-        <v>1766</v>
+        <v>1763</v>
       </c>
       <c r="D1886" s="10">
         <v>3</v>
@@ -67395,7 +67362,7 @@
         <v>16</v>
       </c>
       <c r="H1886" s="8" t="s">
-        <v>1767</v>
+        <v>1764</v>
       </c>
       <c r="I1886" s="4" t="s">
         <v>261</v>
@@ -67422,7 +67389,7 @@
       <c r="F1887" s="13"/>
       <c r="G1887" s="13"/>
       <c r="H1887" s="1" t="s">
-        <v>1724</v>
+        <v>1721</v>
       </c>
       <c r="I1887" s="4" t="s">
         <v>261</v>
@@ -67447,7 +67414,7 @@
         <v>82</v>
       </c>
       <c r="H1888" s="1" t="s">
-        <v>1724</v>
+        <v>1721</v>
       </c>
       <c r="I1888" s="4" t="s">
         <v>261</v>
@@ -67470,7 +67437,7 @@
       <c r="F1889" s="13"/>
       <c r="G1889" s="13"/>
       <c r="H1889" s="1" t="s">
-        <v>1768</v>
+        <v>1765</v>
       </c>
       <c r="I1889" s="13"/>
       <c r="J1889" s="13"/>
@@ -67483,10 +67450,10 @@
         <v>2192</v>
       </c>
       <c r="B1890" s="8" t="s">
-        <v>1769</v>
+        <v>1766</v>
       </c>
       <c r="C1890" s="8" t="s">
-        <v>1770</v>
+        <v>1767</v>
       </c>
       <c r="D1890" s="10">
         <v>3</v>
@@ -67501,7 +67468,7 @@
         <v>16</v>
       </c>
       <c r="H1890" s="9" t="s">
-        <v>1771</v>
+        <v>1768</v>
       </c>
       <c r="I1890" s="4" t="s">
         <v>103</v>
@@ -67524,10 +67491,10 @@
         <v>2448</v>
       </c>
       <c r="B1891" s="8" t="s">
-        <v>1772</v>
+        <v>1769</v>
       </c>
       <c r="C1891" s="9" t="s">
-        <v>1773</v>
+        <v>1770</v>
       </c>
       <c r="D1891" s="10">
         <v>3</v>
@@ -67542,7 +67509,7 @@
         <v>16</v>
       </c>
       <c r="H1891" s="8" t="s">
-        <v>1774</v>
+        <v>1771</v>
       </c>
       <c r="I1891" s="4" t="s">
         <v>103</v>
@@ -67569,7 +67536,7 @@
       <c r="F1892" s="13"/>
       <c r="G1892" s="13"/>
       <c r="H1892" s="1" t="s">
-        <v>1714</v>
+        <v>1711</v>
       </c>
       <c r="I1892" s="4" t="s">
         <v>103</v>
@@ -67588,7 +67555,7 @@
         <v>1683</v>
       </c>
       <c r="B1893" s="1" t="s">
-        <v>1775</v>
+        <v>1772</v>
       </c>
       <c r="C1893" s="1" t="s">
         <v>491</v>
@@ -67604,7 +67571,7 @@
       </c>
       <c r="G1893" s="13"/>
       <c r="H1893" s="1" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="I1893" s="13"/>
       <c r="J1893" s="13"/>
@@ -67617,7 +67584,7 @@
         <v>1751</v>
       </c>
       <c r="B1894" s="1" t="s">
-        <v>1776</v>
+        <v>1773</v>
       </c>
       <c r="C1894" s="1" t="s">
         <v>491</v>
@@ -67633,7 +67600,7 @@
       </c>
       <c r="G1894" s="13"/>
       <c r="H1894" s="1" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="I1894" s="13"/>
       <c r="J1894" s="13"/>
@@ -67646,7 +67613,7 @@
         <v>1700</v>
       </c>
       <c r="B1895" s="1" t="s">
-        <v>1777</v>
+        <v>1774</v>
       </c>
       <c r="C1895" s="1" t="s">
         <v>494</v>
@@ -67675,7 +67642,7 @@
         <v>1767</v>
       </c>
       <c r="B1896" s="1" t="s">
-        <v>1778</v>
+        <v>1775</v>
       </c>
       <c r="C1896" s="1" t="s">
         <v>494</v>
@@ -67704,10 +67671,10 @@
         <v>1497</v>
       </c>
       <c r="B1897" s="8" t="s">
-        <v>1779</v>
+        <v>1776</v>
       </c>
       <c r="C1897" s="9" t="s">
-        <v>1780</v>
+        <v>1777</v>
       </c>
       <c r="D1897" s="10">
         <v>3</v>
@@ -67722,7 +67689,7 @@
         <v>16</v>
       </c>
       <c r="H1897" s="8" t="s">
-        <v>1781</v>
+        <v>1778</v>
       </c>
       <c r="I1897" s="4" t="s">
         <v>103</v>
@@ -67749,7 +67716,7 @@
       <c r="F1898" s="13"/>
       <c r="G1898" s="13"/>
       <c r="H1898" s="1" t="s">
-        <v>1782</v>
+        <v>1779</v>
       </c>
       <c r="I1898" s="4" t="s">
         <v>103</v>
@@ -67768,10 +67735,10 @@
         <v>1498</v>
       </c>
       <c r="B1899" s="8" t="s">
-        <v>1783</v>
+        <v>1780</v>
       </c>
       <c r="C1899" s="9" t="s">
-        <v>1784</v>
+        <v>1781</v>
       </c>
       <c r="D1899" s="10">
         <v>3</v>
@@ -67786,7 +67753,7 @@
         <v>16</v>
       </c>
       <c r="H1899" s="8" t="s">
-        <v>1785</v>
+        <v>1782</v>
       </c>
       <c r="I1899" s="4" t="s">
         <v>84</v>
@@ -67809,10 +67776,10 @@
         <v>1504</v>
       </c>
       <c r="B1900" s="8" t="s">
-        <v>1786</v>
+        <v>1783</v>
       </c>
       <c r="C1900" s="8" t="s">
-        <v>1787</v>
+        <v>1784</v>
       </c>
       <c r="D1900" s="10">
         <v>3</v>
@@ -67827,7 +67794,7 @@
         <v>16</v>
       </c>
       <c r="H1900" s="9" t="s">
-        <v>1788</v>
+        <v>1785</v>
       </c>
       <c r="I1900" s="4" t="s">
         <v>84</v>
@@ -67850,10 +67817,10 @@
         <v>1505</v>
       </c>
       <c r="B1901" s="8" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="C1901" s="9" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="D1901" s="10">
         <v>3</v>
@@ -67868,7 +67835,7 @@
         <v>16</v>
       </c>
       <c r="H1901" s="8" t="s">
-        <v>1791</v>
+        <v>1788</v>
       </c>
       <c r="I1901" s="4" t="s">
         <v>84</v>
@@ -67914,10 +67881,10 @@
         <v>1509</v>
       </c>
       <c r="B1903" s="8" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
       <c r="C1903" s="9" t="s">
-        <v>1793</v>
+        <v>1790</v>
       </c>
       <c r="D1903" s="10">
         <v>3</v>
@@ -67932,7 +67899,7 @@
         <v>16</v>
       </c>
       <c r="H1903" s="8" t="s">
-        <v>1794</v>
+        <v>1791</v>
       </c>
       <c r="I1903" s="4" t="s">
         <v>96</v>
@@ -67955,10 +67922,10 @@
         <v>12327</v>
       </c>
       <c r="B1904" s="8" t="s">
-        <v>1795</v>
+        <v>1792</v>
       </c>
       <c r="C1904" s="9" t="s">
-        <v>1796</v>
+        <v>1793</v>
       </c>
       <c r="D1904" s="10">
         <v>3</v>
@@ -67973,7 +67940,7 @@
         <v>16</v>
       </c>
       <c r="H1904" s="8" t="s">
-        <v>1797</v>
+        <v>1794</v>
       </c>
       <c r="I1904" s="4" t="s">
         <v>96</v>

</xml_diff>